<commit_message>
Updated Mass Properties following Flight 2
update included repair mass and updated ballast based on component
weighing and longitudinal CG balance.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Mass Properties.xlsx
+++ b/Design/CAD/mAEWing1 - Mass Properties.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="460" windowWidth="25440" windowHeight="14580"/>
+    <workbookView xWindow="-255" yWindow="465" windowWidth="25440" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="g">'Components and Fixtures'!$C$2</definedName>
     <definedName name="in2m">'Components and Fixtures'!$C$3</definedName>
   </definedNames>
-  <calcPr calcId="130407"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="151">
   <si>
     <t>Run 4</t>
   </si>
@@ -450,23 +450,61 @@
   <si>
     <t>Roll (Bifilar)</t>
   </si>
+  <si>
+    <t>Left Body Flap</t>
+  </si>
+  <si>
+    <t>Right Body Flap</t>
+  </si>
+  <si>
+    <t>[57.13]</t>
+  </si>
+  <si>
+    <t>[56.35]</t>
+  </si>
+  <si>
+    <t>Summary based on Complete Mass Property Test</t>
+  </si>
+  <si>
+    <t>[119.55]</t>
+  </si>
+  <si>
+    <t>Avionics Battery</t>
+  </si>
+  <si>
+    <t>Propulsion Battery</t>
+  </si>
+  <si>
+    <t>[210.42]</t>
+  </si>
+  <si>
+    <t>[78]</t>
+  </si>
+  <si>
+    <t>[546.64]</t>
+  </si>
+  <si>
+    <t>Added Repair Mass</t>
+  </si>
+  <si>
+    <t>Mass estimated from change in component weight. Position estimate by visual refernce. Neglect body inertia.</t>
+  </si>
+  <si>
+    <t>Summary based on Weight and Balance (Aircraft xCG) following repairs after Flight 2</t>
+  </si>
+  <si>
+    <t>Balance performed to establish required ballast mass.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
-    <numFmt numFmtId="178" formatCode="0.0000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,8 +555,15 @@
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,7 +602,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -914,10 +965,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1039,10 +1091,10 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1063,7 +1115,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1077,7 +1129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1086,7 +1138,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1116,7 +1168,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,7 +1243,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1209,7 +1261,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1227,7 +1279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1239,10 +1291,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1251,7 +1303,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1296,6 +1348,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1305,13 +1367,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1338,25 +1406,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -1381,8 +1471,8 @@
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="329321"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1657,7 +1747,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1839,8 +1929,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="314060"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2034,7 +2124,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2116,8 +2206,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="300019"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2370,7 +2460,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2512,8 +2602,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3848100" cy="563744"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -2933,7 +3023,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -3045,8 +3135,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3848100" cy="563744"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -3466,7 +3556,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -3655,8 +3745,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="474361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -3883,7 +3973,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -3990,8 +4080,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="555793"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -4230,7 +4320,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -4343,8 +4433,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="474361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -4571,7 +4661,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -4678,8 +4768,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="474361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -4906,7 +4996,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -5018,8 +5108,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="463204"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -5215,7 +5305,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -5340,8 +5430,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="463204"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -5537,7 +5627,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -5662,8 +5752,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2771775" cy="474361"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -5890,7 +5980,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -6278,35 +6368,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="4"/>
-      <c r="D1" s="192" t="s">
+      <c r="D1" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="193"/>
-      <c r="F1" s="194"/>
-      <c r="G1" s="192" t="s">
+      <c r="E1" s="197"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="193"/>
-      <c r="I1" s="194"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="H1" s="197"/>
+      <c r="I1" s="198"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="36" t="s">
         <v>108</v>
       </c>
@@ -6332,7 +6422,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="145">
         <v>42161</v>
       </c>
@@ -6340,38 +6430,38 @@
         <v>42</v>
       </c>
       <c r="C3">
-        <f>'Test Summary'!B13</f>
+        <f>'Test Summary'!B18</f>
         <v>6269.81</v>
       </c>
       <c r="D3" s="146">
-        <f>'Test Summary'!C13</f>
+        <f>'Test Summary'!C18</f>
         <v>-23.225000000000001</v>
       </c>
       <c r="E3" s="146">
-        <f>'Test Summary'!D13</f>
+        <f>'Test Summary'!D18</f>
         <v>0</v>
       </c>
       <c r="F3" s="146">
-        <f>'Test Summary'!E13</f>
+        <f>'Test Summary'!E18</f>
         <v>-0.49249999999999994</v>
       </c>
       <c r="G3" s="147">
-        <f>'Test Summary'!F13</f>
+        <f>'Test Summary'!F18</f>
         <v>3.0977856600061244</v>
       </c>
       <c r="H3" s="147">
-        <f>'Test Summary'!G13</f>
+        <f>'Test Summary'!G18</f>
         <v>0.46361697672372681</v>
       </c>
       <c r="I3" s="147">
-        <f>'Test Summary'!H13</f>
+        <f>'Test Summary'!H18</f>
         <v>3.3146271438643926</v>
       </c>
       <c r="J3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="145">
         <v>42161</v>
       </c>
@@ -6407,7 +6497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="145"/>
       <c r="B6" t="s">
         <v>41</v>
@@ -6441,13 +6531,13 @@
         <v>3.289775999932294</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="145"/>
       <c r="D7" s="146"/>
       <c r="E7" s="146"/>
       <c r="F7" s="146"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="145">
         <v>42161</v>
       </c>
@@ -6476,7 +6566,7 @@
         <v>8.8159999999999996E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="145"/>
       <c r="B9" t="s">
         <v>41</v>
@@ -6510,13 +6600,13 @@
         <v>3.2745599661398908</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="145"/>
       <c r="D10" s="146"/>
       <c r="E10" s="146"/>
       <c r="F10" s="146"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="145">
         <v>42166</v>
       </c>
@@ -6550,7 +6640,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="145"/>
       <c r="B12" t="s">
         <v>41</v>
@@ -6584,13 +6674,13 @@
         <v>3.2776814949989417</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="145"/>
       <c r="D13" s="146"/>
       <c r="E13" s="146"/>
       <c r="F13" s="146"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="145">
         <v>42166</v>
       </c>
@@ -6628,7 +6718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="145"/>
       <c r="B15" t="s">
         <v>41</v>
@@ -6662,10 +6752,10 @@
         <v>3.2862816561838057</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="145"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="145">
         <v>42170</v>
       </c>
@@ -6700,7 +6790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -6733,7 +6823,7 @@
         <v>3.3241973978789954</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="145">
         <v>42170</v>
       </c>
@@ -6765,7 +6855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>41</v>
       </c>
@@ -6798,7 +6888,7 @@
         <v>3.3219897911594889</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="145">
         <v>42170</v>
       </c>
@@ -6833,7 +6923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -6866,7 +6956,7 @@
         <v>3.3274354014587431</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="145">
         <v>42170</v>
       </c>
@@ -6904,7 +6994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -6937,7 +7027,7 @@
         <v>3.2903800550582329</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="145">
         <v>42177</v>
       </c>
@@ -6953,7 +7043,7 @@
       <c r="E29" s="146">
         <v>-1.5</v>
       </c>
-      <c r="F29" s="211">
+      <c r="F29" s="195">
         <v>-1.5</v>
       </c>
       <c r="G29" s="146">
@@ -6972,7 +7062,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -7005,7 +7095,7 @@
         <v>3.2873925843392571</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="145">
         <v>42177</v>
       </c>
@@ -7021,7 +7111,7 @@
       <c r="E32" s="146">
         <v>-5.5</v>
       </c>
-      <c r="F32" s="211">
+      <c r="F32" s="195">
         <v>-1.25</v>
       </c>
       <c r="G32" s="146">
@@ -7040,7 +7130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>41</v>
       </c>
@@ -7072,9 +7162,157 @@
         <f>(I30+($C30/1000)*(($D30*in2m-$D33*in2m)^2+($E30*in2m-$E33*in2m)^2)) + SIGN($C32)*((I32)+ABS($C32/1000)*(($D32*in2m-$D33*in2m)^2+($E32*in2m-$E33*in2m)^2))</f>
         <v>3.2885036236808043</v>
       </c>
-      <c r="K33" t="s">
+      <c r="J33" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="145">
+        <v>42186</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35">
+        <v>68.02</v>
+      </c>
+      <c r="D35">
+        <v>-22</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36">
+        <f>C33+C35</f>
+        <v>6565.3100000000013</v>
+      </c>
+      <c r="D36" s="146">
+        <f>(D33*$C33 + D35*$C35)/$C36</f>
+        <v>-23.564105221230982</v>
+      </c>
+      <c r="E36" s="146">
+        <f t="shared" ref="E36:F36" si="18">(E33*$C33 + E35*$C35)/$C36</f>
+        <v>-3.3509461091707778E-2</v>
+      </c>
+      <c r="F36" s="146">
+        <f t="shared" si="18"/>
+        <v>-0.49176374687562335</v>
+      </c>
+      <c r="G36" s="147">
+        <f>(G33+($C33/1000)*(($E33*in2m-$E36*in2m)^2+($F33*in2m-$F36*in2m)^2)) + SIGN($C35)*((G35)+ABS($C35/1000)*(($E35*in2m-$E36*in2m)^2+($F35*in2m-$F36*in2m)^2))</f>
+        <v>3.0985955942841277</v>
+      </c>
+      <c r="H36" s="147">
+        <f>(H33+($C33/1000)*(($D33*in2m-$D36*in2m)^2+($F33*in2m-$F36*in2m)^2)) + SIGN($C35)*((H35)+ABS($C35/1000)*(($D35*in2m-$D36*in2m)^2+($F35*in2m-$F36*in2m)^2))</f>
+        <v>0.43670243136687792</v>
+      </c>
+      <c r="I36" s="147">
+        <f>(I33+($C33/1000)*(($D33*in2m-$D36*in2m)^2+($E33*in2m-$E36*in2m)^2)) + SIGN($C35)*((I35)+ABS($C35/1000)*(($D35*in2m-$D36*in2m)^2+($E35*in2m-$E36*in2m)^2))</f>
+        <v>3.2886121557965287</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="145">
+        <v>42186</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>119.55</v>
+      </c>
+      <c r="D38">
+        <v>-4.62</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>-0.9</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39">
+        <f>C36+C38</f>
+        <v>6684.8600000000015</v>
+      </c>
+      <c r="D39" s="146">
+        <f>(D36*$C36 + D38*$C38)/$C39</f>
+        <v>-23.225314613918609</v>
+      </c>
+      <c r="E39" s="146">
+        <f t="shared" ref="E39:F39" si="19">(E36*$C36 + E38*$C38)/$C39</f>
+        <v>-3.2910188096684147E-2</v>
+      </c>
+      <c r="F39" s="146">
+        <f t="shared" si="19"/>
+        <v>-0.49906451967580451</v>
+      </c>
+      <c r="G39" s="147">
+        <f>(G36+($C36/1000)*(($E36*in2m-$E39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((G38)+ABS($C38/1000)*(($E38*in2m-$E39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
+        <v>3.0986083035190108</v>
+      </c>
+      <c r="H39" s="147">
+        <f>(H36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((H38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
+        <v>0.46389997992190185</v>
+      </c>
+      <c r="I39" s="147">
+        <f>(I36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($E36*in2m-$E39*in2m)^2)) + SIGN($C38)*((I38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($E38*in2m-$E39*in2m)^2))</f>
+        <v>3.3157971652325342</v>
+      </c>
+      <c r="J39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="225">
+        <f>C39/1000*2.20462</f>
+        <v>14.737576053200002</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="226"/>
+      <c r="G42" s="226"/>
+      <c r="H42" s="226"/>
+      <c r="I42" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7093,42 +7331,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C40" sqref="B40:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J2">
         <v>3417.1718982090001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1"/>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="220" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="192" t="s">
+      <c r="C4" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="193"/>
-      <c r="E4" s="194"/>
-      <c r="F4" s="192" t="s">
+      <c r="D4" s="197"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="193"/>
-      <c r="H4" s="194"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
+      <c r="G4" s="197"/>
+      <c r="H4" s="198"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="76"/>
       <c r="B5" s="36" t="s">
         <v>108</v>
@@ -7152,7 +7394,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="118" t="s">
         <v>31</v>
       </c>
@@ -7184,201 +7426,641 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="129">
-        <f>'Components and Fixtures'!C18</f>
-        <v>1407.45</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="129" t="str">
+        <f>'Components and Fixtures'!C17</f>
+        <v>[109.34]</v>
       </c>
       <c r="C7" s="130">
-        <f>'Components and Fixtures'!D18</f>
-        <v>-28.265099212856772</v>
+        <f>'Components and Fixtures'!D17</f>
+        <v>-4.62</v>
       </c>
       <c r="D7" s="131">
-        <f>'Components and Fixtures'!E18</f>
-        <v>-31.416080260883309</v>
-      </c>
-      <c r="E7" s="132" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
-      <c r="H7" s="134"/>
-    </row>
-    <row r="8" spans="1:10">
+        <f>'Components and Fixtures'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="132">
+        <f>'Components and Fixtures'!F17</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F7" s="215"/>
+      <c r="G7" s="215"/>
+      <c r="H7" s="216"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="129">
-        <f>'Components and Fixtures'!C19</f>
-        <v>1432.8</v>
+        <v>142</v>
+      </c>
+      <c r="B8" s="129" t="s">
+        <v>145</v>
       </c>
       <c r="C8" s="130">
-        <f>'Components and Fixtures'!D19</f>
-        <v>-28.405576685387736</v>
+        <f>'Components and Fixtures'!D17</f>
+        <v>-4.62</v>
       </c>
       <c r="D8" s="131">
-        <f>'Components and Fixtures'!E19</f>
-        <v>31.763774206345854</v>
-      </c>
-      <c r="E8" s="132" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="134"/>
-    </row>
-    <row r="9" spans="1:10">
+        <f>'Components and Fixtures'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="132">
+        <f>'Components and Fixtures'!F17</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F8" s="215"/>
+      <c r="G8" s="215"/>
+      <c r="H8" s="216"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="129">
-        <f>'Components and Fixtures'!C20</f>
-        <v>95.85</v>
+        <v>143</v>
+      </c>
+      <c r="B9" s="129" t="s">
+        <v>144</v>
       </c>
       <c r="C9" s="130">
-        <f>'Components and Fixtures'!D20</f>
-        <v>-42.45</v>
+        <v>-19.28</v>
       </c>
       <c r="D9" s="131">
-        <f>'Components and Fixtures'!E20</f>
-        <v>-60.25</v>
+        <v>0</v>
       </c>
       <c r="E9" s="132">
-        <f>'Components and Fixtures'!F20</f>
-        <v>-0.2122</v>
-      </c>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="134"/>
-    </row>
-    <row r="10" spans="1:10">
+        <v>-0.85099999999999998</v>
+      </c>
+      <c r="F9" s="215"/>
+      <c r="G9" s="215"/>
+      <c r="H9" s="216"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="129">
-        <f>'Components and Fixtures'!C21</f>
-        <v>96.45</v>
-      </c>
-      <c r="C10" s="130">
-        <f>'Components and Fixtures'!D21</f>
-        <v>-42.45</v>
-      </c>
-      <c r="D10" s="131">
-        <f>'Components and Fixtures'!E21</f>
-        <v>60.25</v>
-      </c>
-      <c r="E10" s="132">
-        <f>'Components and Fixtures'!F21</f>
-        <v>-0.2122</v>
-      </c>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="134"/>
-    </row>
-    <row r="11" spans="1:10">
+        <v>136</v>
+      </c>
+      <c r="B10" s="129" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="130"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="215"/>
+      <c r="G10" s="215"/>
+      <c r="H10" s="216"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="129">
-        <f>'Components and Fixtures'!C22</f>
-        <v>67.81</v>
+        <v>137</v>
+      </c>
+      <c r="B11" s="129" t="s">
+        <v>139</v>
       </c>
       <c r="C11" s="130"/>
       <c r="D11" s="131"/>
       <c r="E11" s="132"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="134"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
-      <c r="A12" s="77"/>
-      <c r="B12" s="129"/>
-      <c r="C12" s="130"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
+      <c r="F11" s="215"/>
+      <c r="G11" s="215"/>
+      <c r="H11" s="216"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="129">
+        <f>'Components and Fixtures'!C18</f>
+        <v>1407.45</v>
+      </c>
+      <c r="C12" s="130">
+        <f>'Components and Fixtures'!D18</f>
+        <v>-28.265099212856772</v>
+      </c>
+      <c r="D12" s="131">
+        <f>'Components and Fixtures'!E18</f>
+        <v>-31.416080260883309</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>103</v>
+      </c>
       <c r="F12" s="133"/>
       <c r="G12" s="133"/>
       <c r="H12" s="134"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
-      <c r="A13" s="122" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="129">
+        <f>'Components and Fixtures'!C19</f>
+        <v>1432.8</v>
+      </c>
+      <c r="C13" s="130">
+        <f>'Components and Fixtures'!D19</f>
+        <v>-28.405576685387736</v>
+      </c>
+      <c r="D13" s="131">
+        <f>'Components and Fixtures'!E19</f>
+        <v>31.763774206345854</v>
+      </c>
+      <c r="E13" s="132" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="133"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="134"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="129">
+        <f>'Components and Fixtures'!C20</f>
+        <v>95.85</v>
+      </c>
+      <c r="C14" s="130">
+        <f>'Components and Fixtures'!D20</f>
+        <v>-42.45</v>
+      </c>
+      <c r="D14" s="131">
+        <f>'Components and Fixtures'!E20</f>
+        <v>-60.25</v>
+      </c>
+      <c r="E14" s="132">
+        <f>'Components and Fixtures'!F20</f>
+        <v>-0.2122</v>
+      </c>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="134"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="129">
+        <f>'Components and Fixtures'!C21</f>
+        <v>96.45</v>
+      </c>
+      <c r="C15" s="130">
+        <f>'Components and Fixtures'!D21</f>
+        <v>-42.45</v>
+      </c>
+      <c r="D15" s="131">
+        <f>'Components and Fixtures'!E21</f>
+        <v>60.25</v>
+      </c>
+      <c r="E15" s="132">
+        <f>'Components and Fixtures'!F21</f>
+        <v>-0.2122</v>
+      </c>
+      <c r="F15" s="133"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="134"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="129">
+        <f>'Components and Fixtures'!C22</f>
+        <v>67.81</v>
+      </c>
+      <c r="C16" s="130">
+        <f>'Components and Fixtures'!D22</f>
+        <v>-20.216666666666665</v>
+      </c>
+      <c r="D16" s="131">
+        <f>'Components and Fixtures'!E22</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="132">
+        <f>'Components and Fixtures'!F22</f>
+        <v>-0.15666666666666659</v>
+      </c>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="134"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="77"/>
+      <c r="B17" s="129"/>
+      <c r="C17" s="222"/>
+      <c r="D17" s="223"/>
+      <c r="E17" s="224"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="134"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="122" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="135">
-        <f>'Components and Fixtures'!C24</f>
+      <c r="B18" s="135">
+        <f>SUM(B6:B17)</f>
         <v>6269.81</v>
       </c>
-      <c r="C13" s="136">
+      <c r="C18" s="136">
         <f>'Components and Fixtures'!D24</f>
         <v>-23.225000000000001</v>
       </c>
-      <c r="D13" s="137">
+      <c r="D18" s="137">
         <f>'Components and Fixtures'!E24</f>
         <v>0</v>
       </c>
-      <c r="E13" s="138">
+      <c r="E18" s="138">
         <f>'Components and Fixtures'!F24</f>
         <v>-0.49249999999999994</v>
       </c>
-      <c r="F13" s="139">
+      <c r="F18" s="139">
         <f>'Aircraft Test'!S41</f>
         <v>3.0977856600061244</v>
       </c>
-      <c r="G13" s="139">
+      <c r="G18" s="139">
         <f>'Aircraft Test'!C47</f>
         <v>0.46361697672372681</v>
       </c>
-      <c r="H13" s="140">
+      <c r="H18" s="140">
         <f>'Aircraft Test'!K41</f>
         <v>3.3146271438643926</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1"/>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
-      <c r="A15" s="26" t="s">
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="219"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="144">
-        <f>B13/1000*2.20462</f>
+      <c r="B20" s="144">
+        <f>B18/1000*2.20462</f>
         <v>13.8225485222</v>
       </c>
-      <c r="F15" s="141">
-        <f>F13*$J$2</f>
+      <c r="F20" s="141">
+        <f>F18*$J$2</f>
         <v>10585.666104047748</v>
       </c>
-      <c r="G15" s="142">
-        <f>G13*$J$2</f>
+      <c r="G20" s="142">
+        <f>G18*$J$2</f>
         <v>1584.2589043929354</v>
       </c>
-      <c r="H15" s="143">
-        <f>H13*$J$2</f>
+      <c r="H20" s="143">
+        <f>H18*$J$2</f>
         <v>11326.650729054163</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F21" t="s">
         <v>33</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G21" t="s">
         <v>33</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H21" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="220" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="196" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="197"/>
+      <c r="E24" s="198"/>
+      <c r="F24" s="196" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="197"/>
+      <c r="H24" s="198"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="76"/>
+      <c r="B25" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="192" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="193" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="194" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="192" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="193" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="194" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="118" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="217">
+        <v>3529.28</v>
+      </c>
+      <c r="C26" s="221">
+        <f>C6</f>
+        <v>-18.55</v>
+      </c>
+      <c r="D26" s="125">
+        <f>D6</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="126">
+        <f>E6</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="F26" s="127">
+        <f>F6</f>
+        <v>1.5280065868500196E-2</v>
+      </c>
+      <c r="G26" s="127">
+        <f>G6</f>
+        <v>0.13457839359793833</v>
+      </c>
+      <c r="H26" s="128" t="str">
+        <f>H6</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="218" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="130">
+        <f>'Components and Fixtures'!D17</f>
+        <v>-4.62</v>
+      </c>
+      <c r="D27" s="131">
+        <f>'Components and Fixtures'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="132">
+        <f>'Components and Fixtures'!F17</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F27" s="215"/>
+      <c r="G27" s="215"/>
+      <c r="H27" s="216"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="129" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="130">
+        <f>'Components and Fixtures'!D17</f>
+        <v>-4.62</v>
+      </c>
+      <c r="D28" s="131">
+        <f>'Components and Fixtures'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="132">
+        <f>'Components and Fixtures'!F17</f>
+        <v>-0.9</v>
+      </c>
+      <c r="F28" s="215"/>
+      <c r="G28" s="215"/>
+      <c r="H28" s="216"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="129" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="130">
+        <v>-19.28</v>
+      </c>
+      <c r="D29" s="131">
+        <f>'Components and Fixtures'!E17</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="132">
+        <v>-0.85099999999999998</v>
+      </c>
+      <c r="F29" s="215"/>
+      <c r="G29" s="215"/>
+      <c r="H29" s="216"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="129" t="str">
+        <f>B10</f>
+        <v>[57.13]</v>
+      </c>
+      <c r="C30" s="130"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="215"/>
+      <c r="G30" s="215"/>
+      <c r="H30" s="216"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="129" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="130"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="132"/>
+      <c r="F31" s="215"/>
+      <c r="G31" s="215"/>
+      <c r="H31" s="216"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="218">
+        <v>1442.64</v>
+      </c>
+      <c r="C32" s="130">
+        <f t="shared" ref="C32:E32" si="0">C12</f>
+        <v>-28.265099212856772</v>
+      </c>
+      <c r="D32" s="131">
+        <f t="shared" si="0"/>
+        <v>-31.416080260883309</v>
+      </c>
+      <c r="E32" s="132" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="F32" s="133"/>
+      <c r="G32" s="133"/>
+      <c r="H32" s="134"/>
+      <c r="M32" s="219"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="218">
+        <v>1452.83</v>
+      </c>
+      <c r="C33" s="130">
+        <f t="shared" ref="C33:E33" si="1">C13</f>
+        <v>-28.405576685387736</v>
+      </c>
+      <c r="D33" s="131">
+        <f t="shared" si="1"/>
+        <v>31.763774206345854</v>
+      </c>
+      <c r="E33" s="132" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="F33" s="133"/>
+      <c r="G33" s="133"/>
+      <c r="H33" s="134"/>
+      <c r="M33" s="219"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="129">
+        <f>B14</f>
+        <v>95.85</v>
+      </c>
+      <c r="C34" s="130">
+        <f t="shared" ref="C34:E34" si="2">C14</f>
+        <v>-42.45</v>
+      </c>
+      <c r="D34" s="131">
+        <f t="shared" si="2"/>
+        <v>-60.25</v>
+      </c>
+      <c r="E34" s="132">
+        <f t="shared" si="2"/>
+        <v>-0.2122</v>
+      </c>
+      <c r="F34" s="133"/>
+      <c r="G34" s="133"/>
+      <c r="H34" s="134"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="129">
+        <f t="shared" ref="B35:B36" si="3">B15</f>
+        <v>96.45</v>
+      </c>
+      <c r="C35" s="130">
+        <f t="shared" ref="C35:E36" si="4">C15</f>
+        <v>-42.45</v>
+      </c>
+      <c r="D35" s="131">
+        <f t="shared" si="4"/>
+        <v>60.25</v>
+      </c>
+      <c r="E35" s="132">
+        <f t="shared" si="4"/>
+        <v>-0.2122</v>
+      </c>
+      <c r="F35" s="133"/>
+      <c r="G35" s="133"/>
+      <c r="H35" s="134"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="129">
+        <f t="shared" si="3"/>
+        <v>67.81</v>
+      </c>
+      <c r="C36" s="130">
+        <f t="shared" si="4"/>
+        <v>-20.216666666666665</v>
+      </c>
+      <c r="D36" s="131">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="132">
+        <f t="shared" si="4"/>
+        <v>-0.15666666666666659</v>
+      </c>
+      <c r="F36" s="133"/>
+      <c r="G36" s="133"/>
+      <c r="H36" s="134"/>
+    </row>
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="77"/>
+      <c r="B37" s="129"/>
+      <c r="C37" s="130"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="133"/>
+      <c r="H37" s="134"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="122" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="135">
+        <f>SUM(B26:B37)</f>
+        <v>6684.8600000000006</v>
+      </c>
+      <c r="C38" s="136"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="138"/>
+      <c r="F38" s="139"/>
+      <c r="G38" s="139"/>
+      <c r="H38" s="140"/>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="144">
+        <f>B38/1000*2.20462</f>
+        <v>14.7375760532</v>
+      </c>
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:H4"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7388,33 +8070,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1"/>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="58" t="s">
         <v>108</v>
@@ -7426,14 +8108,14 @@
         <v>12</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="192" t="s">
+      <c r="G5" s="196" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="193"/>
-      <c r="I5" s="193"/>
-      <c r="J5" s="194"/>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+      <c r="H5" s="197"/>
+      <c r="I5" s="197"/>
+      <c r="J5" s="198"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
@@ -7461,7 +8143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="117" t="s">
         <v>14</v>
       </c>
@@ -7491,7 +8173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="117" t="s">
         <v>74</v>
       </c>
@@ -7511,18 +8193,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1"/>
-    <row r="10" spans="1:10" ht="15" thickBot="1"/>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="192" t="s">
+      <c r="C11" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="193"/>
-      <c r="E11" s="194"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+      <c r="D11" s="197"/>
+      <c r="E11" s="198"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="76" t="s">
         <v>98</v>
       </c>
@@ -7539,7 +8221,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>13</v>
       </c>
@@ -7559,7 +8241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="78" t="s">
         <v>18</v>
       </c>
@@ -7594,24 +8276,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.5" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1"/>
-    <row r="2" spans="2:10">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
@@ -7622,7 +8304,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>94</v>
       </c>
@@ -7633,22 +8315,22 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1"/>
-    <row r="6" spans="2:10" ht="15" thickBot="1">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="192" t="s">
+      <c r="D6" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="193"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="192" t="s">
+      <c r="E6" s="197"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="193"/>
-      <c r="I6" s="194"/>
-    </row>
-    <row r="7" spans="2:10" ht="15" thickBot="1">
+      <c r="H6" s="197"/>
+      <c r="I6" s="198"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="76" t="s">
         <v>106</v>
       </c>
@@ -7674,7 +8356,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="77" t="s">
         <v>118</v>
       </c>
@@ -7701,7 +8383,7 @@
         <v>5.3499999999999999E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="77" t="s">
         <v>119</v>
       </c>
@@ -7728,7 +8410,7 @@
         <v>7.4599999999999997E-5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" thickBot="1">
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="78" t="s">
         <v>120</v>
       </c>
@@ -7755,7 +8437,7 @@
         <v>2.0699999999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="175" t="s">
         <v>130</v>
       </c>
@@ -7778,22 +8460,22 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1"/>
-    <row r="14" spans="2:10" ht="15" thickBot="1">
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="192" t="s">
+      <c r="D14" s="196" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="193"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="192" t="s">
+      <c r="E14" s="197"/>
+      <c r="F14" s="198"/>
+      <c r="G14" s="196" t="s">
         <v>117</v>
       </c>
-      <c r="H14" s="193"/>
-      <c r="I14" s="194"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" thickBot="1">
+      <c r="H14" s="197"/>
+      <c r="I14" s="198"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="76" t="s">
         <v>98</v>
       </c>
@@ -7819,7 +8501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="118" t="s">
         <v>54</v>
       </c>
@@ -7844,7 +8526,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="77" t="s">
         <v>26</v>
       </c>
@@ -7867,7 +8549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="77" t="s">
         <v>50</v>
       </c>
@@ -7890,7 +8572,7 @@
       <c r="H18" s="183"/>
       <c r="I18" s="184"/>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="77" t="s">
         <v>51</v>
       </c>
@@ -7914,7 +8596,7 @@
       <c r="H19" s="183"/>
       <c r="I19" s="184"/>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="77" t="s">
         <v>52</v>
       </c>
@@ -7943,7 +8625,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="77" t="s">
         <v>53</v>
       </c>
@@ -7975,7 +8657,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="77" t="s">
         <v>25</v>
       </c>
@@ -8000,7 +8682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="77"/>
       <c r="C23" s="177"/>
       <c r="D23" s="11"/>
@@ -8010,7 +8692,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1">
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="78" t="s">
         <v>81</v>
       </c>
@@ -8033,7 +8715,7 @@
       <c r="H24" s="186"/>
       <c r="I24" s="187"/>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>60</v>
       </c>
@@ -8068,31 +8750,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -8100,46 +8782,46 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15" thickBot="1"/>
-    <row r="3" spans="1:32" ht="18">
-      <c r="B3" s="206" t="s">
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:32" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="199" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="208"/>
-      <c r="J3" s="206" t="s">
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="201"/>
+      <c r="J3" s="199" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="208"/>
-      <c r="R3" s="206" t="s">
+      <c r="K3" s="200"/>
+      <c r="L3" s="200"/>
+      <c r="M3" s="200"/>
+      <c r="N3" s="200"/>
+      <c r="O3" s="200"/>
+      <c r="P3" s="201"/>
+      <c r="R3" s="199" t="s">
         <v>134</v>
       </c>
-      <c r="S3" s="207"/>
-      <c r="T3" s="207"/>
-      <c r="U3" s="207"/>
-      <c r="V3" s="207"/>
-      <c r="W3" s="207"/>
-      <c r="X3" s="208"/>
-      <c r="Z3" s="206" t="s">
+      <c r="S3" s="200"/>
+      <c r="T3" s="200"/>
+      <c r="U3" s="200"/>
+      <c r="V3" s="200"/>
+      <c r="W3" s="200"/>
+      <c r="X3" s="201"/>
+      <c r="Z3" s="199" t="s">
         <v>135</v>
       </c>
-      <c r="AA3" s="207"/>
-      <c r="AB3" s="207"/>
-      <c r="AC3" s="207"/>
-      <c r="AD3" s="207"/>
-      <c r="AE3" s="207"/>
-      <c r="AF3" s="208"/>
-    </row>
-    <row r="4" spans="1:32">
+      <c r="AA3" s="200"/>
+      <c r="AB3" s="200"/>
+      <c r="AC3" s="200"/>
+      <c r="AD3" s="200"/>
+      <c r="AE3" s="200"/>
+      <c r="AF3" s="201"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
@@ -8169,101 +8851,101 @@
       <c r="AE4" s="8"/>
       <c r="AF4" s="9"/>
     </row>
-    <row r="5" spans="1:32" ht="15" thickBot="1">
-      <c r="B5" s="198" t="s">
+    <row r="5" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="199"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="200"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
+      <c r="G5" s="205"/>
+      <c r="H5" s="206"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="198" t="s">
+      <c r="J5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="199"/>
-      <c r="L5" s="199"/>
-      <c r="M5" s="199"/>
-      <c r="N5" s="199"/>
-      <c r="O5" s="199"/>
-      <c r="P5" s="200"/>
-      <c r="R5" s="198" t="s">
+      <c r="K5" s="205"/>
+      <c r="L5" s="205"/>
+      <c r="M5" s="205"/>
+      <c r="N5" s="205"/>
+      <c r="O5" s="205"/>
+      <c r="P5" s="206"/>
+      <c r="R5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="199"/>
-      <c r="T5" s="199"/>
-      <c r="U5" s="199"/>
-      <c r="V5" s="199"/>
-      <c r="W5" s="199"/>
-      <c r="X5" s="200"/>
-      <c r="Z5" s="198" t="s">
+      <c r="S5" s="205"/>
+      <c r="T5" s="205"/>
+      <c r="U5" s="205"/>
+      <c r="V5" s="205"/>
+      <c r="W5" s="205"/>
+      <c r="X5" s="206"/>
+      <c r="Z5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="AA5" s="199"/>
-      <c r="AB5" s="199"/>
-      <c r="AC5" s="199"/>
-      <c r="AD5" s="199"/>
-      <c r="AE5" s="199"/>
-      <c r="AF5" s="200"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" thickBot="1">
+      <c r="AA5" s="205"/>
+      <c r="AB5" s="205"/>
+      <c r="AC5" s="205"/>
+      <c r="AD5" s="205"/>
+      <c r="AE5" s="205"/>
+      <c r="AF5" s="206"/>
+    </row>
+    <row r="6" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="201" t="s">
+      <c r="C6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="202"/>
-      <c r="E6" s="203"/>
+      <c r="D6" s="208"/>
+      <c r="E6" s="209"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="204" t="s">
+      <c r="G6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="205"/>
+      <c r="H6" s="211"/>
       <c r="I6" s="10"/>
       <c r="J6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="201" t="s">
+      <c r="K6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="202"/>
-      <c r="M6" s="203"/>
+      <c r="L6" s="208"/>
+      <c r="M6" s="209"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="204" t="s">
+      <c r="O6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="205"/>
+      <c r="P6" s="211"/>
       <c r="R6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="201" t="s">
+      <c r="S6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="T6" s="202"/>
-      <c r="U6" s="203"/>
+      <c r="T6" s="208"/>
+      <c r="U6" s="209"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="204" t="s">
+      <c r="W6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="X6" s="205"/>
+      <c r="X6" s="211"/>
       <c r="Z6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="AA6" s="201" t="s">
+      <c r="AA6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="AB6" s="202"/>
-      <c r="AC6" s="203"/>
+      <c r="AB6" s="208"/>
+      <c r="AC6" s="209"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="204" t="s">
+      <c r="AE6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="AF6" s="205"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" thickBot="1">
+      <c r="AF6" s="211"/>
+    </row>
+    <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="43">
         <v>10</v>
       </c>
@@ -8342,7 +9024,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15" thickBot="1">
+    <row r="8" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>84</v>
       </c>
@@ -8420,7 +9102,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
@@ -8478,7 +9160,7 @@
       <c r="AE9" s="8"/>
       <c r="AF9" s="9"/>
     </row>
-    <row r="10" spans="1:32" ht="15" thickBot="1">
+    <row r="10" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>86</v>
       </c>
@@ -8537,35 +9219,35 @@
       <c r="AE10" s="8"/>
       <c r="AF10" s="9"/>
     </row>
-    <row r="11" spans="1:32" ht="15" thickBot="1">
+    <row r="11" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="204" t="s">
+      <c r="G11" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="205"/>
+      <c r="H11" s="211"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="204" t="s">
+      <c r="O11" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="205"/>
+      <c r="P11" s="211"/>
       <c r="R11" s="11"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="204" t="s">
+      <c r="W11" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="X11" s="205"/>
+      <c r="X11" s="211"/>
       <c r="Z11" s="23" t="s">
         <v>0</v>
       </c>
@@ -8578,7 +9260,7 @@
       <c r="AE11" s="8"/>
       <c r="AF11" s="9"/>
     </row>
-    <row r="12" spans="1:32" ht="15" thickBot="1">
+    <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
         <v>90</v>
       </c>
@@ -8654,12 +9336,12 @@
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8"/>
-      <c r="AE12" s="204" t="s">
+      <c r="AE12" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="AF12" s="205"/>
-    </row>
-    <row r="13" spans="1:32" ht="15" thickBot="1">
+      <c r="AF12" s="211"/>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
         <v>91</v>
       </c>
@@ -8748,7 +9430,7 @@
         <v>1.1834319526627219</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="15" thickBot="1">
+    <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="67"/>
       <c r="C14" s="68"/>
       <c r="D14" s="68"/>
@@ -8789,35 +9471,35 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15" thickBot="1">
-      <c r="B15" s="195" t="s">
+    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="196"/>
-      <c r="D15" s="196"/>
-      <c r="E15" s="196"/>
-      <c r="F15" s="196"/>
-      <c r="G15" s="196"/>
-      <c r="H15" s="197"/>
+      <c r="C15" s="213"/>
+      <c r="D15" s="213"/>
+      <c r="E15" s="213"/>
+      <c r="F15" s="213"/>
+      <c r="G15" s="213"/>
+      <c r="H15" s="214"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="195" t="s">
+      <c r="J15" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="196"/>
-      <c r="L15" s="196"/>
-      <c r="M15" s="196"/>
-      <c r="N15" s="196"/>
-      <c r="O15" s="196"/>
-      <c r="P15" s="197"/>
-      <c r="R15" s="195" t="s">
+      <c r="K15" s="213"/>
+      <c r="L15" s="213"/>
+      <c r="M15" s="213"/>
+      <c r="N15" s="213"/>
+      <c r="O15" s="213"/>
+      <c r="P15" s="214"/>
+      <c r="R15" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="S15" s="196"/>
-      <c r="T15" s="196"/>
-      <c r="U15" s="196"/>
-      <c r="V15" s="196"/>
-      <c r="W15" s="196"/>
-      <c r="X15" s="197"/>
+      <c r="S15" s="213"/>
+      <c r="T15" s="213"/>
+      <c r="U15" s="213"/>
+      <c r="V15" s="213"/>
+      <c r="W15" s="213"/>
+      <c r="X15" s="214"/>
       <c r="Z15" s="38"/>
       <c r="AA15" s="17"/>
       <c r="AB15" s="17"/>
@@ -8826,7 +9508,7 @@
       <c r="AE15" s="17"/>
       <c r="AF15" s="63"/>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B16" s="38"/>
       <c r="C16" s="17" t="s">
         <v>71</v>
@@ -8867,17 +9549,17 @@
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="63"/>
-      <c r="Z16" s="195" t="s">
+      <c r="Z16" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="AA16" s="196"/>
-      <c r="AB16" s="196"/>
-      <c r="AC16" s="196"/>
-      <c r="AD16" s="196"/>
-      <c r="AE16" s="196"/>
-      <c r="AF16" s="197"/>
-    </row>
-    <row r="17" spans="2:32">
+      <c r="AA16" s="213"/>
+      <c r="AB16" s="213"/>
+      <c r="AC16" s="213"/>
+      <c r="AD16" s="213"/>
+      <c r="AE16" s="213"/>
+      <c r="AF16" s="214"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>111</v>
       </c>
@@ -8925,7 +9607,7 @@
       <c r="AE17" s="17"/>
       <c r="AF17" s="63"/>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B18" s="11" t="s">
         <v>112</v>
       </c>
@@ -8975,7 +9657,7 @@
       <c r="AE18" s="17"/>
       <c r="AF18" s="63"/>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>113</v>
       </c>
@@ -9026,7 +9708,7 @@
       <c r="AE19" s="17"/>
       <c r="AF19" s="63"/>
     </row>
-    <row r="20" spans="2:32">
+    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -9072,7 +9754,7 @@
       <c r="AE20" s="17"/>
       <c r="AF20" s="63"/>
     </row>
-    <row r="21" spans="2:32" ht="15" thickBot="1">
+    <row r="21" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>114</v>
       </c>
@@ -9118,7 +9800,7 @@
       <c r="AE21" s="17"/>
       <c r="AF21" s="63"/>
     </row>
-    <row r="22" spans="2:32">
+    <row r="22" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -9161,7 +9843,7 @@
       <c r="AE22" s="17"/>
       <c r="AF22" s="63"/>
     </row>
-    <row r="23" spans="2:32" ht="15" thickBot="1">
+    <row r="23" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>104</v>
       </c>
@@ -9205,7 +9887,7 @@
       <c r="AE23" s="17"/>
       <c r="AF23" s="63"/>
     </row>
-    <row r="24" spans="2:32">
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>68</v>
       </c>
@@ -9227,15 +9909,15 @@
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="63"/>
-      <c r="R24" s="195" t="s">
+      <c r="R24" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="S24" s="196"/>
-      <c r="T24" s="196"/>
-      <c r="U24" s="196"/>
-      <c r="V24" s="196"/>
-      <c r="W24" s="196"/>
-      <c r="X24" s="197"/>
+      <c r="S24" s="213"/>
+      <c r="T24" s="213"/>
+      <c r="U24" s="213"/>
+      <c r="V24" s="213"/>
+      <c r="W24" s="213"/>
+      <c r="X24" s="214"/>
       <c r="Z24" s="38"/>
       <c r="AA24" s="17"/>
       <c r="AB24" s="17"/>
@@ -9244,7 +9926,7 @@
       <c r="AE24" s="17"/>
       <c r="AF24" s="63"/>
     </row>
-    <row r="25" spans="2:32" ht="15" thickBot="1">
+    <row r="25" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
@@ -9293,7 +9975,7 @@
       <c r="AE25" s="17"/>
       <c r="AF25" s="63"/>
     </row>
-    <row r="26" spans="2:32" ht="15" thickBot="1">
+    <row r="26" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -9301,15 +9983,15 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="9"/>
-      <c r="J26" s="195" t="s">
+      <c r="J26" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="K26" s="196"/>
-      <c r="L26" s="196"/>
-      <c r="M26" s="196"/>
-      <c r="N26" s="196"/>
-      <c r="O26" s="196"/>
-      <c r="P26" s="197"/>
+      <c r="K26" s="213"/>
+      <c r="L26" s="213"/>
+      <c r="M26" s="213"/>
+      <c r="N26" s="213"/>
+      <c r="O26" s="213"/>
+      <c r="P26" s="214"/>
       <c r="R26" s="11" t="s">
         <v>114</v>
       </c>
@@ -9341,12 +10023,12 @@
       <c r="AE26" s="17"/>
       <c r="AF26" s="63"/>
     </row>
-    <row r="27" spans="2:32">
-      <c r="B27" s="209" t="s">
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B27" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="210"/>
-      <c r="D27" s="210"/>
+      <c r="C27" s="203"/>
+      <c r="D27" s="203"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -9397,17 +10079,17 @@
         <f>T27+(S27/1000)*(W27*'Components and Fixtures'!$C$3)^2</f>
         <v>1.4701404705388886E-2</v>
       </c>
-      <c r="Z27" s="195" t="s">
+      <c r="Z27" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="AA27" s="196"/>
-      <c r="AB27" s="196"/>
-      <c r="AC27" s="196"/>
-      <c r="AD27" s="196"/>
-      <c r="AE27" s="196"/>
-      <c r="AF27" s="197"/>
-    </row>
-    <row r="28" spans="2:32" ht="15" thickBot="1">
+      <c r="AA27" s="213"/>
+      <c r="AB27" s="213"/>
+      <c r="AC27" s="213"/>
+      <c r="AD27" s="213"/>
+      <c r="AE27" s="213"/>
+      <c r="AF27" s="214"/>
+    </row>
+    <row r="28" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="61" t="s">
         <v>62</v>
       </c>
@@ -9480,7 +10162,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="2:32">
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
       <c r="J29" s="11" t="s">
         <v>106</v>
       </c>
@@ -9539,7 +10221,7 @@
         <v>1.121180353715957E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:32">
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
       <c r="J30" s="11" t="s">
         <v>98</v>
       </c>
@@ -9602,7 +10284,7 @@
         <v>1.6143585024029996E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:32">
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
       <c r="J31" s="11"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -9630,7 +10312,7 @@
       <c r="AE31" s="57"/>
       <c r="AF31" s="65"/>
     </row>
-    <row r="32" spans="2:32" ht="15" thickBot="1">
+    <row r="32" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J32" s="11" t="s">
         <v>81</v>
       </c>
@@ -9678,7 +10360,7 @@
       <c r="AE32" s="8"/>
       <c r="AF32" s="9"/>
     </row>
-    <row r="33" spans="10:32" ht="15" thickBot="1">
+    <row r="33" spans="10:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J33" s="11"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -9706,7 +10388,7 @@
       <c r="AE33" s="57"/>
       <c r="AF33" s="65"/>
     </row>
-    <row r="34" spans="10:32" ht="15" thickBot="1">
+    <row r="34" spans="10:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J34" s="12" t="str">
         <f>J30</f>
         <v>Body</v>
@@ -9748,7 +10430,7 @@
       <c r="AE34" s="2"/>
       <c r="AF34" s="4"/>
     </row>
-    <row r="35" spans="10:32">
+    <row r="35" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J35" s="1"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -9785,7 +10467,7 @@
       <c r="AE35" s="8"/>
       <c r="AF35" s="9"/>
     </row>
-    <row r="36" spans="10:32">
+    <row r="36" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J36" s="5" t="s">
         <v>104</v>
       </c>
@@ -9829,7 +10511,7 @@
       <c r="AE36" s="8"/>
       <c r="AF36" s="9"/>
     </row>
-    <row r="37" spans="10:32">
+    <row r="37" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J37" s="5" t="s">
         <v>68</v>
       </c>
@@ -9866,7 +10548,7 @@
       <c r="AE37" s="8"/>
       <c r="AF37" s="9"/>
     </row>
-    <row r="38" spans="10:32">
+    <row r="38" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J38" s="5" t="s">
         <v>32</v>
       </c>
@@ -9881,11 +10563,11 @@
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
       <c r="P38" s="9"/>
-      <c r="R38" s="209" t="s">
+      <c r="R38" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="S38" s="210"/>
-      <c r="T38" s="210"/>
+      <c r="S38" s="203"/>
+      <c r="T38" s="203"/>
       <c r="U38" s="8"/>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
@@ -9905,7 +10587,7 @@
       <c r="AE38" s="8"/>
       <c r="AF38" s="9"/>
     </row>
-    <row r="39" spans="10:32">
+    <row r="39" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J39" s="11"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -9935,12 +10617,12 @@
       <c r="AE39" s="8"/>
       <c r="AF39" s="9"/>
     </row>
-    <row r="40" spans="10:32">
-      <c r="J40" s="209" t="s">
+    <row r="40" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="J40" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="K40" s="210"/>
-      <c r="L40" s="210"/>
+      <c r="K40" s="203"/>
+      <c r="L40" s="203"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -9952,17 +10634,17 @@
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
       <c r="X40" s="9"/>
-      <c r="Z40" s="209" t="s">
+      <c r="Z40" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="AA40" s="210"/>
-      <c r="AB40" s="210"/>
+      <c r="AA40" s="203"/>
+      <c r="AB40" s="203"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
       <c r="AF40" s="9"/>
     </row>
-    <row r="41" spans="10:32">
+    <row r="41" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J41" s="90" t="s">
         <v>62</v>
       </c>
@@ -9977,11 +10659,11 @@
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="9"/>
-      <c r="R41" s="209" t="s">
+      <c r="R41" s="202" t="s">
         <v>129</v>
       </c>
-      <c r="S41" s="210"/>
-      <c r="T41" s="210"/>
+      <c r="S41" s="203"/>
+      <c r="T41" s="203"/>
       <c r="U41" s="8"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
@@ -10001,7 +10683,7 @@
       <c r="AE41" s="8"/>
       <c r="AF41" s="9"/>
     </row>
-    <row r="42" spans="10:32">
+    <row r="42" spans="10:32" x14ac:dyDescent="0.25">
       <c r="J42" s="11"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -10031,12 +10713,12 @@
       <c r="AE42" s="8"/>
       <c r="AF42" s="9"/>
     </row>
-    <row r="43" spans="10:32">
-      <c r="J43" s="209" t="s">
+    <row r="43" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="J43" s="202" t="s">
         <v>129</v>
       </c>
-      <c r="K43" s="210"/>
-      <c r="L43" s="210"/>
+      <c r="K43" s="203"/>
+      <c r="L43" s="203"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -10048,17 +10730,17 @@
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
       <c r="X43" s="9"/>
-      <c r="Z43" s="209" t="s">
+      <c r="Z43" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="AA43" s="210"/>
-      <c r="AB43" s="210"/>
+      <c r="AA43" s="203"/>
+      <c r="AB43" s="203"/>
       <c r="AC43" s="8"/>
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
       <c r="AF43" s="9"/>
     </row>
-    <row r="44" spans="10:32" ht="15" thickBot="1">
+    <row r="44" spans="10:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J44" s="90" t="s">
         <v>62</v>
       </c>
@@ -10073,11 +10755,11 @@
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
       <c r="P44" s="9"/>
-      <c r="R44" s="209" t="s">
+      <c r="R44" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="S44" s="210"/>
-      <c r="T44" s="210"/>
+      <c r="S44" s="203"/>
+      <c r="T44" s="203"/>
       <c r="U44" s="8"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
@@ -10097,7 +10779,7 @@
       <c r="AE44" s="13"/>
       <c r="AF44" s="15"/>
     </row>
-    <row r="45" spans="10:32" ht="15" thickBot="1">
+    <row r="45" spans="10:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J45" s="11"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
@@ -10120,18 +10802,18 @@
       <c r="W45" s="13"/>
       <c r="X45" s="15"/>
     </row>
-    <row r="46" spans="10:32">
-      <c r="J46" s="209" t="s">
+    <row r="46" spans="10:32" x14ac:dyDescent="0.25">
+      <c r="J46" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="K46" s="210"/>
-      <c r="L46" s="210"/>
+      <c r="K46" s="203"/>
+      <c r="L46" s="203"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
       <c r="P46" s="9"/>
     </row>
-    <row r="47" spans="10:32" ht="15" thickBot="1">
+    <row r="47" spans="10:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J47" s="61" t="s">
         <v>62</v>
       </c>
@@ -10149,20 +10831,12 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="Z27:AF27"/>
+    <mergeCell ref="Z5:AF5"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="Z16:AF16"/>
     <mergeCell ref="Z3:AF3"/>
     <mergeCell ref="J46:L46"/>
     <mergeCell ref="R3:X3"/>
@@ -10179,12 +10853,20 @@
     <mergeCell ref="R44:T44"/>
     <mergeCell ref="Z40:AB40"/>
     <mergeCell ref="Z43:AB43"/>
-    <mergeCell ref="Z27:AF27"/>
-    <mergeCell ref="Z5:AF5"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="Z16:AF16"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J5:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10197,21 +10879,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -10219,37 +10901,37 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15" thickBot="1"/>
-    <row r="3" spans="1:24" ht="18">
-      <c r="B3" s="206" t="s">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:24" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="208"/>
-      <c r="J3" s="206" t="s">
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="201"/>
+      <c r="J3" s="199" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
-      <c r="P3" s="208"/>
-      <c r="R3" s="206" t="s">
+      <c r="K3" s="200"/>
+      <c r="L3" s="200"/>
+      <c r="M3" s="200"/>
+      <c r="N3" s="200"/>
+      <c r="O3" s="200"/>
+      <c r="P3" s="201"/>
+      <c r="R3" s="199" t="s">
         <v>135</v>
       </c>
-      <c r="S3" s="207"/>
-      <c r="T3" s="207"/>
-      <c r="U3" s="207"/>
-      <c r="V3" s="207"/>
-      <c r="W3" s="207"/>
-      <c r="X3" s="208"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="S3" s="200"/>
+      <c r="T3" s="200"/>
+      <c r="U3" s="200"/>
+      <c r="V3" s="200"/>
+      <c r="W3" s="200"/>
+      <c r="X3" s="201"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
@@ -10272,77 +10954,77 @@
       <c r="W4" s="8"/>
       <c r="X4" s="9"/>
     </row>
-    <row r="5" spans="1:24" ht="15" thickBot="1">
-      <c r="B5" s="198" t="s">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="199"/>
-      <c r="D5" s="199"/>
-      <c r="E5" s="199"/>
-      <c r="F5" s="199"/>
-      <c r="G5" s="199"/>
-      <c r="H5" s="200"/>
-      <c r="J5" s="198" t="s">
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
+      <c r="G5" s="205"/>
+      <c r="H5" s="206"/>
+      <c r="J5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="199"/>
-      <c r="L5" s="199"/>
-      <c r="M5" s="199"/>
-      <c r="N5" s="199"/>
-      <c r="O5" s="199"/>
-      <c r="P5" s="200"/>
-      <c r="R5" s="198" t="s">
+      <c r="K5" s="205"/>
+      <c r="L5" s="205"/>
+      <c r="M5" s="205"/>
+      <c r="N5" s="205"/>
+      <c r="O5" s="205"/>
+      <c r="P5" s="206"/>
+      <c r="R5" s="204" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="199"/>
-      <c r="T5" s="199"/>
-      <c r="U5" s="199"/>
-      <c r="V5" s="199"/>
-      <c r="W5" s="199"/>
-      <c r="X5" s="200"/>
-    </row>
-    <row r="6" spans="1:24" ht="15" thickBot="1">
+      <c r="S5" s="205"/>
+      <c r="T5" s="205"/>
+      <c r="U5" s="205"/>
+      <c r="V5" s="205"/>
+      <c r="W5" s="205"/>
+      <c r="X5" s="206"/>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="201" t="s">
+      <c r="C6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="202"/>
-      <c r="E6" s="202"/>
+      <c r="D6" s="208"/>
+      <c r="E6" s="208"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="204" t="s">
+      <c r="G6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="205"/>
+      <c r="H6" s="211"/>
       <c r="J6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="201" t="s">
+      <c r="K6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="202"/>
-      <c r="M6" s="203"/>
+      <c r="L6" s="208"/>
+      <c r="M6" s="209"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="204" t="s">
+      <c r="O6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="205"/>
+      <c r="P6" s="211"/>
       <c r="R6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="201" t="s">
+      <c r="S6" s="207" t="s">
         <v>100</v>
       </c>
-      <c r="T6" s="202"/>
-      <c r="U6" s="203"/>
+      <c r="T6" s="208"/>
+      <c r="U6" s="209"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="204" t="s">
+      <c r="W6" s="210" t="s">
         <v>101</v>
       </c>
-      <c r="X6" s="205"/>
-    </row>
-    <row r="7" spans="1:24" ht="15" thickBot="1">
+      <c r="X6" s="211"/>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="43">
         <v>20</v>
       </c>
@@ -10398,7 +11080,7 @@
         <v>57.496666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15" thickBot="1">
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>84</v>
       </c>
@@ -10455,7 +11137,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
@@ -10496,7 +11178,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="9"/>
     </row>
-    <row r="10" spans="1:24" ht="15" thickBot="1">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
         <v>86</v>
       </c>
@@ -10537,7 +11219,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="9"/>
     </row>
-    <row r="11" spans="1:24" ht="15" thickBot="1">
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>0</v>
       </c>
@@ -10561,30 +11243,30 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="204" t="s">
+      <c r="O11" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="205"/>
+      <c r="P11" s="211"/>
       <c r="R11" s="11"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="204" t="s">
+      <c r="W11" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="X11" s="205"/>
-    </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1">
+      <c r="X11" s="211"/>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="204" t="s">
+      <c r="G12" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="205"/>
+      <c r="H12" s="211"/>
       <c r="J12" s="24" t="s">
         <v>90</v>
       </c>
@@ -10620,7 +11302,7 @@
         <v>0.17392312597831761</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="15" thickBot="1">
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="24" t="s">
         <v>90</v>
       </c>
@@ -10682,7 +11364,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="15" thickBot="1">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
         <v>91</v>
       </c>
@@ -10724,7 +11406,7 @@
       <c r="W14" s="17"/>
       <c r="X14" s="63"/>
     </row>
-    <row r="15" spans="1:24" ht="15" thickBot="1">
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="38"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -10732,35 +11414,35 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="63"/>
-      <c r="J15" s="195" t="s">
+      <c r="J15" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="196"/>
-      <c r="L15" s="196"/>
-      <c r="M15" s="196"/>
-      <c r="N15" s="196"/>
-      <c r="O15" s="196"/>
-      <c r="P15" s="197"/>
-      <c r="R15" s="195" t="s">
+      <c r="K15" s="213"/>
+      <c r="L15" s="213"/>
+      <c r="M15" s="213"/>
+      <c r="N15" s="213"/>
+      <c r="O15" s="213"/>
+      <c r="P15" s="214"/>
+      <c r="R15" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="S15" s="196"/>
-      <c r="T15" s="196"/>
-      <c r="U15" s="196"/>
-      <c r="V15" s="196"/>
-      <c r="W15" s="196"/>
-      <c r="X15" s="197"/>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="B16" s="195" t="s">
+      <c r="S15" s="213"/>
+      <c r="T15" s="213"/>
+      <c r="U15" s="213"/>
+      <c r="V15" s="213"/>
+      <c r="W15" s="213"/>
+      <c r="X15" s="214"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="212" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="196"/>
-      <c r="D16" s="196"/>
-      <c r="E16" s="196"/>
-      <c r="F16" s="196"/>
-      <c r="G16" s="196"/>
-      <c r="H16" s="197"/>
+      <c r="C16" s="213"/>
+      <c r="D16" s="213"/>
+      <c r="E16" s="213"/>
+      <c r="F16" s="213"/>
+      <c r="G16" s="213"/>
+      <c r="H16" s="214"/>
       <c r="J16" s="38" t="s">
         <v>1</v>
       </c>
@@ -10788,7 +11470,7 @@
       <c r="W16" s="17"/>
       <c r="X16" s="63"/>
     </row>
-    <row r="17" spans="2:24">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
         <v>9</v>
       </c>
@@ -10829,7 +11511,7 @@
       <c r="W17" s="17"/>
       <c r="X17" s="63"/>
     </row>
-    <row r="18" spans="2:24">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
         <v>10</v>
       </c>
@@ -10870,7 +11552,7 @@
       <c r="W18" s="17"/>
       <c r="X18" s="63"/>
     </row>
-    <row r="19" spans="2:24">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="38"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -10905,7 +11587,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="63"/>
     </row>
-    <row r="20" spans="2:24">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>125</v>
       </c>
@@ -10934,7 +11616,7 @@
       <c r="W20" s="17"/>
       <c r="X20" s="63"/>
     </row>
-    <row r="21" spans="2:24">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
         <v>126</v>
       </c>
@@ -10976,7 +11658,7 @@
       <c r="W21" s="17"/>
       <c r="X21" s="63"/>
     </row>
-    <row r="22" spans="2:24">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B22" s="89">
         <f>-46.07+C18</f>
         <v>-45.837000000000003</v>
@@ -11017,7 +11699,7 @@
       <c r="W22" s="17"/>
       <c r="X22" s="63"/>
     </row>
-    <row r="23" spans="2:24" ht="15" thickBot="1">
+    <row r="23" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="32"/>
@@ -11040,7 +11722,7 @@
       <c r="W23" s="17"/>
       <c r="X23" s="63"/>
     </row>
-    <row r="24" spans="2:24">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="8"/>
       <c r="D24" s="17"/>
@@ -11048,26 +11730,26 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
       <c r="H24" s="63"/>
-      <c r="J24" s="195" t="s">
+      <c r="J24" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="K24" s="196"/>
-      <c r="L24" s="196"/>
-      <c r="M24" s="196"/>
-      <c r="N24" s="196"/>
-      <c r="O24" s="196"/>
-      <c r="P24" s="197"/>
-      <c r="R24" s="195" t="s">
+      <c r="K24" s="213"/>
+      <c r="L24" s="213"/>
+      <c r="M24" s="213"/>
+      <c r="N24" s="213"/>
+      <c r="O24" s="213"/>
+      <c r="P24" s="214"/>
+      <c r="R24" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="S24" s="196"/>
-      <c r="T24" s="196"/>
-      <c r="U24" s="196"/>
-      <c r="V24" s="196"/>
-      <c r="W24" s="196"/>
-      <c r="X24" s="197"/>
-    </row>
-    <row r="25" spans="2:24" ht="15" thickBot="1">
+      <c r="S24" s="213"/>
+      <c r="T24" s="213"/>
+      <c r="U24" s="213"/>
+      <c r="V24" s="213"/>
+      <c r="W24" s="213"/>
+      <c r="X24" s="214"/>
+    </row>
+    <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11"/>
       <c r="C25" s="8"/>
       <c r="D25" s="17"/>
@@ -11114,16 +11796,16 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="2:24">
-      <c r="B26" s="195" t="s">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="212" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="196"/>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196"/>
-      <c r="F26" s="196"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="197"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="213"/>
+      <c r="E26" s="213"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="214"/>
       <c r="J26" s="11" t="s">
         <v>114</v>
       </c>
@@ -11171,7 +11853,7 @@
         <v>1.2232662240775781E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:24">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B27" s="38"/>
       <c r="C27" s="17" t="s">
         <v>71</v>
@@ -11244,7 +11926,7 @@
         <v>6.485994009611998E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:24">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>114</v>
       </c>
@@ -11285,7 +11967,7 @@
       <c r="W28" s="57"/>
       <c r="X28" s="65"/>
     </row>
-    <row r="29" spans="2:24">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>106</v>
       </c>
@@ -11328,7 +12010,7 @@
       <c r="W29" s="8"/>
       <c r="X29" s="9"/>
     </row>
-    <row r="30" spans="2:24" ht="15" thickBot="1">
+    <row r="30" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="11" t="s">
         <v>98</v>
       </c>
@@ -11375,7 +12057,7 @@
       <c r="W30" s="57"/>
       <c r="X30" s="65"/>
     </row>
-    <row r="31" spans="2:24">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="11"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -11398,7 +12080,7 @@
       <c r="W31" s="2"/>
       <c r="X31" s="4"/>
     </row>
-    <row r="32" spans="2:24">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>81</v>
       </c>
@@ -11448,7 +12130,7 @@
       <c r="W32" s="8"/>
       <c r="X32" s="9"/>
     </row>
-    <row r="33" spans="2:24">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="11"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -11485,7 +12167,7 @@
       <c r="W33" s="8"/>
       <c r="X33" s="9"/>
     </row>
-    <row r="34" spans="2:24" ht="15" thickBot="1">
+    <row r="34" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="str">
         <f>B30</f>
         <v>Body</v>
@@ -11534,7 +12216,7 @@
       <c r="W34" s="8"/>
       <c r="X34" s="9"/>
     </row>
-    <row r="35" spans="2:24">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -11571,7 +12253,7 @@
       <c r="W35" s="8"/>
       <c r="X35" s="9"/>
     </row>
-    <row r="36" spans="2:24">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>104</v>
       </c>
@@ -11601,7 +12283,7 @@
       <c r="W36" s="8"/>
       <c r="X36" s="9"/>
     </row>
-    <row r="37" spans="2:24">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>68</v>
       </c>
@@ -11616,26 +12298,26 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
-      <c r="J37" s="209" t="s">
+      <c r="J37" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="K37" s="210"/>
-      <c r="L37" s="210"/>
+      <c r="K37" s="203"/>
+      <c r="L37" s="203"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
       <c r="P37" s="9"/>
-      <c r="R37" s="209" t="s">
+      <c r="R37" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="S37" s="210"/>
-      <c r="T37" s="210"/>
+      <c r="S37" s="203"/>
+      <c r="T37" s="203"/>
       <c r="U37" s="8"/>
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
       <c r="X37" s="9"/>
     </row>
-    <row r="38" spans="2:24">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>105</v>
       </c>
@@ -11679,7 +12361,7 @@
       <c r="W38" s="8"/>
       <c r="X38" s="9"/>
     </row>
-    <row r="39" spans="2:24">
+    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -11702,36 +12384,36 @@
       <c r="W39" s="8"/>
       <c r="X39" s="9"/>
     </row>
-    <row r="40" spans="2:24">
-      <c r="B40" s="209" t="s">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B40" s="202" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="210"/>
-      <c r="D40" s="210"/>
+      <c r="C40" s="203"/>
+      <c r="D40" s="203"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="9"/>
-      <c r="J40" s="209" t="s">
+      <c r="J40" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="K40" s="210"/>
-      <c r="L40" s="210"/>
+      <c r="K40" s="203"/>
+      <c r="L40" s="203"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="9"/>
-      <c r="R40" s="209" t="s">
+      <c r="R40" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="S40" s="210"/>
-      <c r="T40" s="210"/>
+      <c r="S40" s="203"/>
+      <c r="T40" s="203"/>
       <c r="U40" s="8"/>
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
       <c r="X40" s="9"/>
     </row>
-    <row r="41" spans="2:24" ht="15" thickBot="1">
+    <row r="41" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="90" t="s">
         <v>62</v>
       </c>
@@ -11775,7 +12457,7 @@
       <c r="W41" s="13"/>
       <c r="X41" s="15"/>
     </row>
-    <row r="42" spans="2:24">
+    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -11784,18 +12466,18 @@
       <c r="G42" s="8"/>
       <c r="H42" s="9"/>
     </row>
-    <row r="43" spans="2:24">
-      <c r="B43" s="209" t="s">
+    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B43" s="202" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="210"/>
-      <c r="D43" s="210"/>
+      <c r="C43" s="203"/>
+      <c r="D43" s="203"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="2:24">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B44" s="90" t="s">
         <v>62</v>
       </c>
@@ -11811,7 +12493,7 @@
       <c r="G44" s="8"/>
       <c r="H44" s="9"/>
     </row>
-    <row r="45" spans="2:24">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -11820,18 +12502,18 @@
       <c r="G45" s="8"/>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="2:24">
-      <c r="B46" s="209" t="s">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B46" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="210"/>
-      <c r="D46" s="210"/>
+      <c r="C46" s="203"/>
+      <c r="D46" s="203"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
       <c r="H46" s="9"/>
     </row>
-    <row r="47" spans="2:24" ht="15" thickBot="1">
+    <row r="47" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="61" t="s">
         <v>62</v>
       </c>
@@ -11849,16 +12531,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="R37:T37"/>
+    <mergeCell ref="R40:T40"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J40:L40"/>
     <mergeCell ref="R15:X15"/>
     <mergeCell ref="R24:X24"/>
     <mergeCell ref="J3:P3"/>
@@ -11872,11 +12549,16 @@
     <mergeCell ref="S6:U6"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="R37:T37"/>
-    <mergeCell ref="R40:T40"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Mirror Left Wing to Right Wing
Mirror to populate the accel brackets from the left wing to the right
wing.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Mass Properties.xlsx
+++ b/Design/CAD/mAEWing1 - Mass Properties.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-255" yWindow="465" windowWidth="25440" windowHeight="14580"/>
@@ -18,7 +18,7 @@
     <definedName name="g">'Components and Fixtures'!$C$2</definedName>
     <definedName name="in2m">'Components and Fixtures'!$C$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="154">
   <si>
     <t>Run 4</t>
   </si>
@@ -495,6 +495,15 @@
   <si>
     <t>Balance performed to establish required ballast mass.</t>
   </si>
+  <si>
+    <t>Reduced Ballast</t>
+  </si>
+  <si>
+    <t>Rewiring Flight Computer</t>
+  </si>
+  <si>
+    <t>Mass estimated based on position estimate and ballast required to balance</t>
+  </si>
 </sst>
 </file>
 
@@ -504,7 +513,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,13 +563,6 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -965,11 +967,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1358,63 +1359,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1442,11 +1386,66 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -1514,7 +1513,7 @@
                     <m:sSubSupPr>
                       <m:ctrlPr>
                         <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
                       </m:ctrlPr>
                     </m:sSubSupPr>
@@ -1557,7 +1556,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -1626,7 +1625,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -1691,7 +1690,7 @@
                             <a:schemeClr val="tx1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="Cambria Math"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -1977,7 +1976,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -2013,7 +2012,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2081,7 +2080,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2258,7 +2257,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2307,7 +2306,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2362,7 +2361,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2417,7 +2416,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2654,7 +2653,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -2699,7 +2698,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -2712,7 +2711,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2755,7 +2754,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2810,7 +2809,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2825,7 +2824,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="Cambria Math"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2908,7 +2907,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -2923,7 +2922,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="Cambria Math"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -2992,7 +2991,7 @@
                           <m:sSubPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSubPr>
@@ -3187,7 +3186,7 @@
                               <a:schemeClr val="tx1"/>
                             </a:solidFill>
                             <a:effectLst/>
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
@@ -3232,7 +3231,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -3245,7 +3244,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3288,7 +3287,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3343,7 +3342,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3358,7 +3357,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="Cambria Math"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -3441,7 +3440,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3456,7 +3455,7 @@
                                       <a:schemeClr val="tx1"/>
                                     </a:solidFill>
                                     <a:effectLst/>
-                                    <a:latin typeface="Cambria Math"/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     <a:ea typeface="+mn-ea"/>
                                     <a:cs typeface="+mn-cs"/>
                                   </a:rPr>
@@ -3525,7 +3524,7 @@
                           <m:sSubPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSubPr>
@@ -3793,7 +3792,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -3832,7 +3831,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -3845,7 +3844,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3900,7 +3899,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -3941,7 +3940,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -4128,7 +4127,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -4167,7 +4166,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -4180,7 +4179,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4235,7 +4234,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4276,7 +4275,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -4481,7 +4480,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -4520,7 +4519,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -4533,7 +4532,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4588,7 +4587,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4629,7 +4628,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -4816,7 +4815,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -4855,7 +4854,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -4868,7 +4867,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4923,7 +4922,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -4964,7 +4963,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -5156,7 +5155,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -5195,7 +5194,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -5208,7 +5207,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -5261,7 +5260,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -5478,7 +5477,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -5517,7 +5516,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -5530,7 +5529,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -5583,7 +5582,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -5800,7 +5799,7 @@
                       <m:sSubSupPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:sSubSupPr>
@@ -5839,7 +5838,7 @@
                       <m:fPr>
                         <m:ctrlPr>
                           <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                            <a:latin typeface="Cambria Math"/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           </a:rPr>
                         </m:ctrlPr>
                       </m:fPr>
@@ -5852,7 +5851,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -5907,7 +5906,7 @@
                                   <a:schemeClr val="tx1"/>
                                 </a:solidFill>
                                 <a:effectLst/>
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                 <a:ea typeface="+mn-ea"/>
                                 <a:cs typeface="+mn-cs"/>
                               </a:rPr>
@@ -5948,7 +5947,7 @@
                           <m:sSupPr>
                             <m:ctrlPr>
                               <a:rPr lang="en-US" sz="1800" b="0" i="1">
-                                <a:latin typeface="Cambria Math"/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                               </a:rPr>
                             </m:ctrlPr>
                           </m:sSupPr>
@@ -6125,7 +6124,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6160,7 +6159,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6369,15 +6368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" customWidth="1"/>
@@ -6385,16 +6385,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="4"/>
-      <c r="D1" s="196" t="s">
+      <c r="D1" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="197"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="196" t="s">
+      <c r="E1" s="208"/>
+      <c r="F1" s="209"/>
+      <c r="G1" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="197"/>
-      <c r="I1" s="198"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="209"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="36" t="s">
@@ -7299,20 +7299,150 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C40" s="225">
-        <f>C39/1000*2.20462</f>
-        <v>14.737576053200002</v>
-      </c>
-      <c r="D40" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="145">
+        <v>42217</v>
+      </c>
+      <c r="B41" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41">
+        <v>95</v>
+      </c>
+      <c r="D41">
+        <f>D38-6</f>
+        <v>-10.620000000000001</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f>F38</f>
+        <v>-0.9</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>C39+C41</f>
+        <v>6779.8600000000015</v>
+      </c>
+      <c r="D42" s="146">
+        <f>(D39*$C39 + D41*$C41)/$C42</f>
+        <v>-23.048687826887274</v>
+      </c>
+      <c r="E42" s="146">
+        <f t="shared" ref="E42:F42" si="20">(E39*$C39 + E41*$C41)/$C42</f>
+        <v>-3.2449047620452337E-2</v>
+      </c>
+      <c r="F42" s="146">
+        <f t="shared" si="20"/>
+        <v>-0.50468246320720467</v>
+      </c>
+      <c r="G42" s="147">
+        <f>(G39+($C39/1000)*(($E39*in2m-$E42*in2m)^2+($F39*in2m-$F42*in2m)^2)) + SIGN($C41)*((G41)+ABS($C41/1000)*(($E41*in2m-$E42*in2m)^2+($F41*in2m-$F42*in2m)^2))</f>
+        <v>3.0986180832732715</v>
+      </c>
+      <c r="H42" s="147">
+        <f>(H39+($C39/1000)*(($D39*in2m-$D42*in2m)^2+($F39*in2m-$F42*in2m)^2)) + SIGN($C41)*((H41)+ABS($C41/1000)*(($D41*in2m-$D42*in2m)^2+($F41*in2m-$F42*in2m)^2))</f>
+        <v>0.47351187787654875</v>
+      </c>
+      <c r="I42" s="147">
+        <f>(I39+($C39/1000)*(($D39*in2m-$D42*in2m)^2+($E39*in2m-$E42*in2m)^2)) + SIGN($C41)*((I41)+ABS($C41/1000)*(($D41*in2m-$D42*in2m)^2+($E41*in2m-$E42*in2m)^2))</f>
+        <v>3.3253994143370518</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="145">
+        <v>42217</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44">
+        <f>49-121</f>
+        <v>-72</v>
+      </c>
+      <c r="D44">
+        <v>-4.62</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>-0.9</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45">
+        <f>C42+C44</f>
+        <v>6707.8600000000015</v>
+      </c>
+      <c r="D45" s="146">
+        <f>(D42*$C42 + D44*$C44)/$C45</f>
+        <v>-23.24649540240851</v>
+      </c>
+      <c r="E45" s="146">
+        <f t="shared" ref="E45:F45" si="21">(E42*$C42 + E44*$C44)/$C45</f>
+        <v>-3.2797345203984578E-2</v>
+      </c>
+      <c r="F45" s="146">
+        <f t="shared" si="21"/>
+        <v>-0.50043925260813416</v>
+      </c>
+      <c r="G45" s="147">
+        <f>(G42+($C42/1000)*(($E42*in2m-$E45*in2m)^2+($F42*in2m-$F45*in2m)^2)) + SIGN($C44)*((G44)+ABS($C44/1000)*(($E44*in2m-$E45*in2m)^2+($F44*in2m-$F45*in2m)^2))</f>
+        <v>3.0986106966634375</v>
+      </c>
+      <c r="H45" s="147">
+        <f>(H42+($C42/1000)*(($D42*in2m-$D45*in2m)^2+($F42*in2m-$F45*in2m)^2)) + SIGN($C44)*((H44)+ABS($C44/1000)*(($D44*in2m-$D45*in2m)^2+($F44*in2m-$F45*in2m)^2))</f>
+        <v>0.45755950512559773</v>
+      </c>
+      <c r="I45" s="147">
+        <f>(I42+($C42/1000)*(($D42*in2m-$D45*in2m)^2+($E42*in2m-$E45*in2m)^2)) + SIGN($C44)*((I44)+ABS($C44/1000)*(($D44*in2m-$D45*in2m)^2+($E44*in2m-$E45*in2m)^2))</f>
+        <v>3.3094543293245606</v>
+      </c>
+      <c r="J45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="206">
+        <f>C45/1000*2.20462</f>
+        <v>14.788282313200003</v>
+      </c>
+      <c r="D49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C42" s="226"/>
-      <c r="G42" s="226"/>
-      <c r="H42" s="226"/>
-      <c r="I42" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7350,7 +7480,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="220" t="s">
+      <c r="A3" s="201" t="s">
         <v>140</v>
       </c>
     </row>
@@ -7359,16 +7489,16 @@
         <v>35</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="196" t="s">
+      <c r="C4" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="197"/>
-      <c r="E4" s="198"/>
-      <c r="F4" s="196" t="s">
+      <c r="D4" s="208"/>
+      <c r="E4" s="209"/>
+      <c r="F4" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="G4" s="197"/>
-      <c r="H4" s="198"/>
+      <c r="G4" s="208"/>
+      <c r="H4" s="209"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="76"/>
@@ -7446,9 +7576,9 @@
         <f>'Components and Fixtures'!F17</f>
         <v>-0.9</v>
       </c>
-      <c r="F7" s="215"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="216"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="196"/>
+      <c r="H7" s="197"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
@@ -7469,9 +7599,9 @@
         <f>'Components and Fixtures'!F17</f>
         <v>-0.9</v>
       </c>
-      <c r="F8" s="215"/>
-      <c r="G8" s="215"/>
-      <c r="H8" s="216"/>
+      <c r="F8" s="196"/>
+      <c r="G8" s="196"/>
+      <c r="H8" s="197"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
@@ -7489,9 +7619,9 @@
       <c r="E9" s="132">
         <v>-0.85099999999999998</v>
       </c>
-      <c r="F9" s="215"/>
-      <c r="G9" s="215"/>
-      <c r="H9" s="216"/>
+      <c r="F9" s="196"/>
+      <c r="G9" s="196"/>
+      <c r="H9" s="197"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="77" t="s">
@@ -7503,9 +7633,9 @@
       <c r="C10" s="130"/>
       <c r="D10" s="131"/>
       <c r="E10" s="132"/>
-      <c r="F10" s="215"/>
-      <c r="G10" s="215"/>
-      <c r="H10" s="216"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="197"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
@@ -7517,9 +7647,9 @@
       <c r="C11" s="130"/>
       <c r="D11" s="131"/>
       <c r="E11" s="132"/>
-      <c r="F11" s="215"/>
-      <c r="G11" s="215"/>
-      <c r="H11" s="216"/>
+      <c r="F11" s="196"/>
+      <c r="G11" s="196"/>
+      <c r="H11" s="197"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
@@ -7642,9 +7772,9 @@
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="77"/>
       <c r="B17" s="129"/>
-      <c r="C17" s="222"/>
-      <c r="D17" s="223"/>
-      <c r="E17" s="224"/>
+      <c r="C17" s="203"/>
+      <c r="D17" s="204"/>
+      <c r="E17" s="205"/>
       <c r="F17" s="133"/>
       <c r="G17" s="133"/>
       <c r="H17" s="134"/>
@@ -7683,7 +7813,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="219"/>
+      <c r="B19" s="200"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
@@ -7721,7 +7851,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="220" t="s">
+      <c r="A23" s="201" t="s">
         <v>149</v>
       </c>
     </row>
@@ -7730,16 +7860,16 @@
         <v>35</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="196" t="s">
+      <c r="C24" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="197"/>
-      <c r="E24" s="198"/>
-      <c r="F24" s="196" t="s">
+      <c r="D24" s="208"/>
+      <c r="E24" s="209"/>
+      <c r="F24" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="G24" s="197"/>
-      <c r="H24" s="198"/>
+      <c r="G24" s="208"/>
+      <c r="H24" s="209"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="76"/>
@@ -7769,31 +7899,31 @@
       <c r="A26" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="217">
+      <c r="B26" s="198">
         <v>3529.28</v>
       </c>
-      <c r="C26" s="221">
-        <f>C6</f>
+      <c r="C26" s="202">
+        <f t="shared" ref="C26:H26" si="0">C6</f>
         <v>-18.55</v>
       </c>
       <c r="D26" s="125">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" s="126">
-        <f>E6</f>
+        <f t="shared" si="0"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="F26" s="127">
-        <f>F6</f>
+        <f t="shared" si="0"/>
         <v>1.5280065868500196E-2</v>
       </c>
       <c r="G26" s="127">
-        <f>G6</f>
+        <f t="shared" si="0"/>
         <v>0.13457839359793833</v>
       </c>
       <c r="H26" s="128" t="str">
-        <f>H6</f>
+        <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
     </row>
@@ -7801,7 +7931,7 @@
       <c r="A27" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="218" t="s">
+      <c r="B27" s="199" t="s">
         <v>141</v>
       </c>
       <c r="C27" s="130">
@@ -7816,9 +7946,9 @@
         <f>'Components and Fixtures'!F17</f>
         <v>-0.9</v>
       </c>
-      <c r="F27" s="215"/>
-      <c r="G27" s="215"/>
-      <c r="H27" s="216"/>
+      <c r="F27" s="196"/>
+      <c r="G27" s="196"/>
+      <c r="H27" s="197"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
@@ -7839,9 +7969,9 @@
         <f>'Components and Fixtures'!F17</f>
         <v>-0.9</v>
       </c>
-      <c r="F28" s="215"/>
-      <c r="G28" s="215"/>
-      <c r="H28" s="216"/>
+      <c r="F28" s="196"/>
+      <c r="G28" s="196"/>
+      <c r="H28" s="197"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="77" t="s">
@@ -7860,9 +7990,9 @@
       <c r="E29" s="132">
         <v>-0.85099999999999998</v>
       </c>
-      <c r="F29" s="215"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="216"/>
+      <c r="F29" s="196"/>
+      <c r="G29" s="196"/>
+      <c r="H29" s="197"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
@@ -7875,9 +8005,9 @@
       <c r="C30" s="130"/>
       <c r="D30" s="131"/>
       <c r="E30" s="132"/>
-      <c r="F30" s="215"/>
-      <c r="G30" s="215"/>
-      <c r="H30" s="216"/>
+      <c r="F30" s="196"/>
+      <c r="G30" s="196"/>
+      <c r="H30" s="197"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="77" t="s">
@@ -7889,57 +8019,57 @@
       <c r="C31" s="130"/>
       <c r="D31" s="131"/>
       <c r="E31" s="132"/>
-      <c r="F31" s="215"/>
-      <c r="G31" s="215"/>
-      <c r="H31" s="216"/>
+      <c r="F31" s="196"/>
+      <c r="G31" s="196"/>
+      <c r="H31" s="197"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="218">
+      <c r="B32" s="199">
         <v>1442.64</v>
       </c>
       <c r="C32" s="130">
-        <f t="shared" ref="C32:E32" si="0">C12</f>
+        <f t="shared" ref="C32:E32" si="1">C12</f>
         <v>-28.265099212856772</v>
       </c>
       <c r="D32" s="131">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-31.416080260883309</v>
       </c>
       <c r="E32" s="132" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
       <c r="F32" s="133"/>
       <c r="G32" s="133"/>
       <c r="H32" s="134"/>
-      <c r="M32" s="219"/>
+      <c r="M32" s="200"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="218">
+      <c r="B33" s="199">
         <v>1452.83</v>
       </c>
       <c r="C33" s="130">
-        <f t="shared" ref="C33:E33" si="1">C13</f>
+        <f t="shared" ref="C33:E33" si="2">C13</f>
         <v>-28.405576685387736</v>
       </c>
       <c r="D33" s="131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31.763774206345854</v>
       </c>
       <c r="E33" s="132" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>N/A</v>
       </c>
       <c r="F33" s="133"/>
       <c r="G33" s="133"/>
       <c r="H33" s="134"/>
-      <c r="M33" s="219"/>
+      <c r="M33" s="200"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="77" t="s">
@@ -7950,15 +8080,15 @@
         <v>95.85</v>
       </c>
       <c r="C34" s="130">
-        <f t="shared" ref="C34:E34" si="2">C14</f>
+        <f t="shared" ref="C34:E34" si="3">C14</f>
         <v>-42.45</v>
       </c>
       <c r="D34" s="131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-60.25</v>
       </c>
       <c r="E34" s="132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.2122</v>
       </c>
       <c r="F34" s="133"/>
@@ -7970,19 +8100,19 @@
         <v>24</v>
       </c>
       <c r="B35" s="129">
-        <f t="shared" ref="B35:B36" si="3">B15</f>
+        <f t="shared" ref="B35:B36" si="4">B15</f>
         <v>96.45</v>
       </c>
       <c r="C35" s="130">
-        <f t="shared" ref="C35:E36" si="4">C15</f>
+        <f t="shared" ref="C35:E36" si="5">C15</f>
         <v>-42.45</v>
       </c>
       <c r="D35" s="131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60.25</v>
       </c>
       <c r="E35" s="132">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.2122</v>
       </c>
       <c r="F35" s="133"/>
@@ -7994,19 +8124,19 @@
         <v>25</v>
       </c>
       <c r="B36" s="129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67.81</v>
       </c>
       <c r="C36" s="130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-20.216666666666665</v>
       </c>
       <c r="D36" s="131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E36" s="132">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.15666666666666659</v>
       </c>
       <c r="F36" s="133"/>
@@ -8108,12 +8238,12 @@
         <v>12</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="196" t="s">
+      <c r="G5" s="207" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="197"/>
-      <c r="I5" s="197"/>
-      <c r="J5" s="198"/>
+      <c r="H5" s="208"/>
+      <c r="I5" s="208"/>
+      <c r="J5" s="209"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
@@ -8198,11 +8328,11 @@
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="196" t="s">
+      <c r="C11" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="197"/>
-      <c r="E11" s="198"/>
+      <c r="D11" s="208"/>
+      <c r="E11" s="209"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="76" t="s">
@@ -8319,16 +8449,16 @@
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="196" t="s">
+      <c r="D6" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="197"/>
-      <c r="F6" s="198"/>
-      <c r="G6" s="196" t="s">
+      <c r="E6" s="208"/>
+      <c r="F6" s="209"/>
+      <c r="G6" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="197"/>
-      <c r="I6" s="198"/>
+      <c r="H6" s="208"/>
+      <c r="I6" s="209"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="76" t="s">
@@ -8464,16 +8594,16 @@
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="196" t="s">
+      <c r="D14" s="207" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="197"/>
-      <c r="F14" s="198"/>
-      <c r="G14" s="196" t="s">
+      <c r="E14" s="208"/>
+      <c r="F14" s="209"/>
+      <c r="G14" s="207" t="s">
         <v>117</v>
       </c>
-      <c r="H14" s="197"/>
-      <c r="I14" s="198"/>
+      <c r="H14" s="208"/>
+      <c r="I14" s="209"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="76" t="s">
@@ -8784,42 +8914,42 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:32" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="221" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201"/>
-      <c r="J3" s="199" t="s">
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="223"/>
+      <c r="J3" s="221" t="s">
         <v>115</v>
       </c>
-      <c r="K3" s="200"/>
-      <c r="L3" s="200"/>
-      <c r="M3" s="200"/>
-      <c r="N3" s="200"/>
-      <c r="O3" s="200"/>
-      <c r="P3" s="201"/>
-      <c r="R3" s="199" t="s">
+      <c r="K3" s="222"/>
+      <c r="L3" s="222"/>
+      <c r="M3" s="222"/>
+      <c r="N3" s="222"/>
+      <c r="O3" s="222"/>
+      <c r="P3" s="223"/>
+      <c r="R3" s="221" t="s">
         <v>134</v>
       </c>
-      <c r="S3" s="200"/>
-      <c r="T3" s="200"/>
-      <c r="U3" s="200"/>
-      <c r="V3" s="200"/>
-      <c r="W3" s="200"/>
-      <c r="X3" s="201"/>
-      <c r="Z3" s="199" t="s">
+      <c r="S3" s="222"/>
+      <c r="T3" s="222"/>
+      <c r="U3" s="222"/>
+      <c r="V3" s="222"/>
+      <c r="W3" s="222"/>
+      <c r="X3" s="223"/>
+      <c r="Z3" s="221" t="s">
         <v>135</v>
       </c>
-      <c r="AA3" s="200"/>
-      <c r="AB3" s="200"/>
-      <c r="AC3" s="200"/>
-      <c r="AD3" s="200"/>
-      <c r="AE3" s="200"/>
-      <c r="AF3" s="201"/>
+      <c r="AA3" s="222"/>
+      <c r="AB3" s="222"/>
+      <c r="AC3" s="222"/>
+      <c r="AD3" s="222"/>
+      <c r="AE3" s="222"/>
+      <c r="AF3" s="223"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -8852,98 +8982,98 @@
       <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="204" t="s">
+      <c r="B5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="206"/>
+      <c r="C5" s="214"/>
+      <c r="D5" s="214"/>
+      <c r="E5" s="214"/>
+      <c r="F5" s="214"/>
+      <c r="G5" s="214"/>
+      <c r="H5" s="215"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="204" t="s">
+      <c r="J5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="205"/>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
-      <c r="O5" s="205"/>
-      <c r="P5" s="206"/>
-      <c r="R5" s="204" t="s">
+      <c r="K5" s="214"/>
+      <c r="L5" s="214"/>
+      <c r="M5" s="214"/>
+      <c r="N5" s="214"/>
+      <c r="O5" s="214"/>
+      <c r="P5" s="215"/>
+      <c r="R5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="205"/>
-      <c r="T5" s="205"/>
-      <c r="U5" s="205"/>
-      <c r="V5" s="205"/>
-      <c r="W5" s="205"/>
-      <c r="X5" s="206"/>
-      <c r="Z5" s="204" t="s">
+      <c r="S5" s="214"/>
+      <c r="T5" s="214"/>
+      <c r="U5" s="214"/>
+      <c r="V5" s="214"/>
+      <c r="W5" s="214"/>
+      <c r="X5" s="215"/>
+      <c r="Z5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="AA5" s="205"/>
-      <c r="AB5" s="205"/>
-      <c r="AC5" s="205"/>
-      <c r="AD5" s="205"/>
-      <c r="AE5" s="205"/>
-      <c r="AF5" s="206"/>
+      <c r="AA5" s="214"/>
+      <c r="AB5" s="214"/>
+      <c r="AC5" s="214"/>
+      <c r="AD5" s="214"/>
+      <c r="AE5" s="214"/>
+      <c r="AF5" s="215"/>
     </row>
     <row r="6" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="207" t="s">
+      <c r="C6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="208"/>
-      <c r="E6" s="209"/>
+      <c r="D6" s="217"/>
+      <c r="E6" s="218"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="210" t="s">
+      <c r="G6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="211"/>
+      <c r="H6" s="220"/>
       <c r="I6" s="10"/>
       <c r="J6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="208"/>
-      <c r="M6" s="209"/>
+      <c r="L6" s="217"/>
+      <c r="M6" s="218"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="210" t="s">
+      <c r="O6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="211"/>
+      <c r="P6" s="220"/>
       <c r="R6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="207" t="s">
+      <c r="S6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="T6" s="208"/>
-      <c r="U6" s="209"/>
+      <c r="T6" s="217"/>
+      <c r="U6" s="218"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="210" t="s">
+      <c r="W6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="X6" s="211"/>
+      <c r="X6" s="220"/>
       <c r="Z6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="AA6" s="207" t="s">
+      <c r="AA6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="AB6" s="208"/>
-      <c r="AC6" s="209"/>
+      <c r="AB6" s="217"/>
+      <c r="AC6" s="218"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="210" t="s">
+      <c r="AE6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="AF6" s="211"/>
+      <c r="AF6" s="220"/>
     </row>
     <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="43">
@@ -9225,29 +9355,29 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="210" t="s">
+      <c r="G11" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="211"/>
+      <c r="H11" s="220"/>
       <c r="I11" s="8"/>
       <c r="J11" s="11"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="210" t="s">
+      <c r="O11" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="211"/>
+      <c r="P11" s="220"/>
       <c r="R11" s="11"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="210" t="s">
+      <c r="W11" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="X11" s="211"/>
+      <c r="X11" s="220"/>
       <c r="Z11" s="23" t="s">
         <v>0</v>
       </c>
@@ -9336,10 +9466,10 @@
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8"/>
-      <c r="AE12" s="210" t="s">
+      <c r="AE12" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="AF12" s="211"/>
+      <c r="AF12" s="220"/>
     </row>
     <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
@@ -9472,34 +9602,34 @@
       </c>
     </row>
     <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="212" t="s">
+      <c r="B15" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="213"/>
-      <c r="D15" s="213"/>
-      <c r="E15" s="213"/>
-      <c r="F15" s="213"/>
-      <c r="G15" s="213"/>
-      <c r="H15" s="214"/>
+      <c r="C15" s="211"/>
+      <c r="D15" s="211"/>
+      <c r="E15" s="211"/>
+      <c r="F15" s="211"/>
+      <c r="G15" s="211"/>
+      <c r="H15" s="212"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="212" t="s">
+      <c r="J15" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="213"/>
-      <c r="L15" s="213"/>
-      <c r="M15" s="213"/>
-      <c r="N15" s="213"/>
-      <c r="O15" s="213"/>
-      <c r="P15" s="214"/>
-      <c r="R15" s="212" t="s">
+      <c r="K15" s="211"/>
+      <c r="L15" s="211"/>
+      <c r="M15" s="211"/>
+      <c r="N15" s="211"/>
+      <c r="O15" s="211"/>
+      <c r="P15" s="212"/>
+      <c r="R15" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="S15" s="213"/>
-      <c r="T15" s="213"/>
-      <c r="U15" s="213"/>
-      <c r="V15" s="213"/>
-      <c r="W15" s="213"/>
-      <c r="X15" s="214"/>
+      <c r="S15" s="211"/>
+      <c r="T15" s="211"/>
+      <c r="U15" s="211"/>
+      <c r="V15" s="211"/>
+      <c r="W15" s="211"/>
+      <c r="X15" s="212"/>
       <c r="Z15" s="38"/>
       <c r="AA15" s="17"/>
       <c r="AB15" s="17"/>
@@ -9549,15 +9679,15 @@
       <c r="V16" s="17"/>
       <c r="W16" s="17"/>
       <c r="X16" s="63"/>
-      <c r="Z16" s="212" t="s">
+      <c r="Z16" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="AA16" s="213"/>
-      <c r="AB16" s="213"/>
-      <c r="AC16" s="213"/>
-      <c r="AD16" s="213"/>
-      <c r="AE16" s="213"/>
-      <c r="AF16" s="214"/>
+      <c r="AA16" s="211"/>
+      <c r="AB16" s="211"/>
+      <c r="AC16" s="211"/>
+      <c r="AD16" s="211"/>
+      <c r="AE16" s="211"/>
+      <c r="AF16" s="212"/>
     </row>
     <row r="17" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
@@ -9909,15 +10039,15 @@
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="63"/>
-      <c r="R24" s="212" t="s">
+      <c r="R24" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="S24" s="213"/>
-      <c r="T24" s="213"/>
-      <c r="U24" s="213"/>
-      <c r="V24" s="213"/>
-      <c r="W24" s="213"/>
-      <c r="X24" s="214"/>
+      <c r="S24" s="211"/>
+      <c r="T24" s="211"/>
+      <c r="U24" s="211"/>
+      <c r="V24" s="211"/>
+      <c r="W24" s="211"/>
+      <c r="X24" s="212"/>
       <c r="Z24" s="38"/>
       <c r="AA24" s="17"/>
       <c r="AB24" s="17"/>
@@ -9983,15 +10113,15 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
       <c r="H26" s="9"/>
-      <c r="J26" s="212" t="s">
+      <c r="J26" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="K26" s="213"/>
-      <c r="L26" s="213"/>
-      <c r="M26" s="213"/>
-      <c r="N26" s="213"/>
-      <c r="O26" s="213"/>
-      <c r="P26" s="214"/>
+      <c r="K26" s="211"/>
+      <c r="L26" s="211"/>
+      <c r="M26" s="211"/>
+      <c r="N26" s="211"/>
+      <c r="O26" s="211"/>
+      <c r="P26" s="212"/>
       <c r="R26" s="11" t="s">
         <v>114</v>
       </c>
@@ -10024,11 +10154,11 @@
       <c r="AF26" s="63"/>
     </row>
     <row r="27" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B27" s="202" t="s">
+      <c r="B27" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="203"/>
-      <c r="D27" s="203"/>
+      <c r="C27" s="225"/>
+      <c r="D27" s="225"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -10079,15 +10209,15 @@
         <f>T27+(S27/1000)*(W27*'Components and Fixtures'!$C$3)^2</f>
         <v>1.4701404705388886E-2</v>
       </c>
-      <c r="Z27" s="212" t="s">
+      <c r="Z27" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="AA27" s="213"/>
-      <c r="AB27" s="213"/>
-      <c r="AC27" s="213"/>
-      <c r="AD27" s="213"/>
-      <c r="AE27" s="213"/>
-      <c r="AF27" s="214"/>
+      <c r="AA27" s="211"/>
+      <c r="AB27" s="211"/>
+      <c r="AC27" s="211"/>
+      <c r="AD27" s="211"/>
+      <c r="AE27" s="211"/>
+      <c r="AF27" s="212"/>
     </row>
     <row r="28" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="61" t="s">
@@ -10563,11 +10693,11 @@
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
       <c r="P38" s="9"/>
-      <c r="R38" s="202" t="s">
+      <c r="R38" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="S38" s="203"/>
-      <c r="T38" s="203"/>
+      <c r="S38" s="225"/>
+      <c r="T38" s="225"/>
       <c r="U38" s="8"/>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
@@ -10618,11 +10748,11 @@
       <c r="AF39" s="9"/>
     </row>
     <row r="40" spans="10:32" x14ac:dyDescent="0.25">
-      <c r="J40" s="202" t="s">
+      <c r="J40" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="K40" s="203"/>
-      <c r="L40" s="203"/>
+      <c r="K40" s="225"/>
+      <c r="L40" s="225"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -10634,11 +10764,11 @@
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
       <c r="X40" s="9"/>
-      <c r="Z40" s="202" t="s">
+      <c r="Z40" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="AA40" s="203"/>
-      <c r="AB40" s="203"/>
+      <c r="AA40" s="225"/>
+      <c r="AB40" s="225"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
@@ -10659,11 +10789,11 @@
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="9"/>
-      <c r="R41" s="202" t="s">
+      <c r="R41" s="224" t="s">
         <v>129</v>
       </c>
-      <c r="S41" s="203"/>
-      <c r="T41" s="203"/>
+      <c r="S41" s="225"/>
+      <c r="T41" s="225"/>
       <c r="U41" s="8"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
@@ -10714,11 +10844,11 @@
       <c r="AF42" s="9"/>
     </row>
     <row r="43" spans="10:32" x14ac:dyDescent="0.25">
-      <c r="J43" s="202" t="s">
+      <c r="J43" s="224" t="s">
         <v>129</v>
       </c>
-      <c r="K43" s="203"/>
-      <c r="L43" s="203"/>
+      <c r="K43" s="225"/>
+      <c r="L43" s="225"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -10730,11 +10860,11 @@
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
       <c r="X43" s="9"/>
-      <c r="Z43" s="202" t="s">
+      <c r="Z43" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="AA43" s="203"/>
-      <c r="AB43" s="203"/>
+      <c r="AA43" s="225"/>
+      <c r="AB43" s="225"/>
       <c r="AC43" s="8"/>
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
@@ -10755,11 +10885,11 @@
       <c r="N44" s="8"/>
       <c r="O44" s="8"/>
       <c r="P44" s="9"/>
-      <c r="R44" s="202" t="s">
+      <c r="R44" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="S44" s="203"/>
-      <c r="T44" s="203"/>
+      <c r="S44" s="225"/>
+      <c r="T44" s="225"/>
       <c r="U44" s="8"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
@@ -10803,11 +10933,11 @@
       <c r="X45" s="15"/>
     </row>
     <row r="46" spans="10:32" x14ac:dyDescent="0.25">
-      <c r="J46" s="202" t="s">
+      <c r="J46" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="K46" s="203"/>
-      <c r="L46" s="203"/>
+      <c r="K46" s="225"/>
+      <c r="L46" s="225"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
@@ -10831,12 +10961,20 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="Z27:AF27"/>
-    <mergeCell ref="Z5:AF5"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="Z16:AF16"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J5:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B15:H15"/>
     <mergeCell ref="Z3:AF3"/>
     <mergeCell ref="J46:L46"/>
     <mergeCell ref="R3:X3"/>
@@ -10853,20 +10991,12 @@
     <mergeCell ref="R44:T44"/>
     <mergeCell ref="Z40:AB40"/>
     <mergeCell ref="Z43:AB43"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="Z27:AF27"/>
+    <mergeCell ref="Z5:AF5"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="Z16:AF16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10903,33 +11033,33 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:24" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="221" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="200"/>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="200"/>
-      <c r="H3" s="201"/>
-      <c r="J3" s="199" t="s">
+      <c r="C3" s="222"/>
+      <c r="D3" s="222"/>
+      <c r="E3" s="222"/>
+      <c r="F3" s="222"/>
+      <c r="G3" s="222"/>
+      <c r="H3" s="223"/>
+      <c r="J3" s="221" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="200"/>
-      <c r="L3" s="200"/>
-      <c r="M3" s="200"/>
-      <c r="N3" s="200"/>
-      <c r="O3" s="200"/>
-      <c r="P3" s="201"/>
-      <c r="R3" s="199" t="s">
+      <c r="K3" s="222"/>
+      <c r="L3" s="222"/>
+      <c r="M3" s="222"/>
+      <c r="N3" s="222"/>
+      <c r="O3" s="222"/>
+      <c r="P3" s="223"/>
+      <c r="R3" s="221" t="s">
         <v>135</v>
       </c>
-      <c r="S3" s="200"/>
-      <c r="T3" s="200"/>
-      <c r="U3" s="200"/>
-      <c r="V3" s="200"/>
-      <c r="W3" s="200"/>
-      <c r="X3" s="201"/>
+      <c r="S3" s="222"/>
+      <c r="T3" s="222"/>
+      <c r="U3" s="222"/>
+      <c r="V3" s="222"/>
+      <c r="W3" s="222"/>
+      <c r="X3" s="223"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
@@ -10955,74 +11085,74 @@
       <c r="X4" s="9"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="204" t="s">
+      <c r="B5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="205"/>
-      <c r="D5" s="205"/>
-      <c r="E5" s="205"/>
-      <c r="F5" s="205"/>
-      <c r="G5" s="205"/>
-      <c r="H5" s="206"/>
-      <c r="J5" s="204" t="s">
+      <c r="C5" s="214"/>
+      <c r="D5" s="214"/>
+      <c r="E5" s="214"/>
+      <c r="F5" s="214"/>
+      <c r="G5" s="214"/>
+      <c r="H5" s="215"/>
+      <c r="J5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="K5" s="205"/>
-      <c r="L5" s="205"/>
-      <c r="M5" s="205"/>
-      <c r="N5" s="205"/>
-      <c r="O5" s="205"/>
-      <c r="P5" s="206"/>
-      <c r="R5" s="204" t="s">
+      <c r="K5" s="214"/>
+      <c r="L5" s="214"/>
+      <c r="M5" s="214"/>
+      <c r="N5" s="214"/>
+      <c r="O5" s="214"/>
+      <c r="P5" s="215"/>
+      <c r="R5" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="205"/>
-      <c r="T5" s="205"/>
-      <c r="U5" s="205"/>
-      <c r="V5" s="205"/>
-      <c r="W5" s="205"/>
-      <c r="X5" s="206"/>
+      <c r="S5" s="214"/>
+      <c r="T5" s="214"/>
+      <c r="U5" s="214"/>
+      <c r="V5" s="214"/>
+      <c r="W5" s="214"/>
+      <c r="X5" s="215"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="207" t="s">
+      <c r="C6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="208"/>
-      <c r="E6" s="208"/>
+      <c r="D6" s="217"/>
+      <c r="E6" s="217"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="210" t="s">
+      <c r="G6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="H6" s="211"/>
+      <c r="H6" s="220"/>
       <c r="J6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="208"/>
-      <c r="M6" s="209"/>
+      <c r="L6" s="217"/>
+      <c r="M6" s="218"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="210" t="s">
+      <c r="O6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="P6" s="211"/>
+      <c r="P6" s="220"/>
       <c r="R6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="207" t="s">
+      <c r="S6" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="T6" s="208"/>
-      <c r="U6" s="209"/>
+      <c r="T6" s="217"/>
+      <c r="U6" s="218"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="210" t="s">
+      <c r="W6" s="219" t="s">
         <v>101</v>
       </c>
-      <c r="X6" s="211"/>
+      <c r="X6" s="220"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="43">
@@ -11243,19 +11373,19 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="210" t="s">
+      <c r="O11" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="P11" s="211"/>
+      <c r="P11" s="220"/>
       <c r="R11" s="11"/>
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
-      <c r="W11" s="210" t="s">
+      <c r="W11" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="X11" s="211"/>
+      <c r="X11" s="220"/>
     </row>
     <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
@@ -11263,10 +11393,10 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="210" t="s">
+      <c r="G12" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="H12" s="211"/>
+      <c r="H12" s="220"/>
       <c r="J12" s="24" t="s">
         <v>90</v>
       </c>
@@ -11414,35 +11544,35 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="63"/>
-      <c r="J15" s="212" t="s">
+      <c r="J15" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="K15" s="213"/>
-      <c r="L15" s="213"/>
-      <c r="M15" s="213"/>
-      <c r="N15" s="213"/>
-      <c r="O15" s="213"/>
-      <c r="P15" s="214"/>
-      <c r="R15" s="212" t="s">
+      <c r="K15" s="211"/>
+      <c r="L15" s="211"/>
+      <c r="M15" s="211"/>
+      <c r="N15" s="211"/>
+      <c r="O15" s="211"/>
+      <c r="P15" s="212"/>
+      <c r="R15" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="S15" s="213"/>
-      <c r="T15" s="213"/>
-      <c r="U15" s="213"/>
-      <c r="V15" s="213"/>
-      <c r="W15" s="213"/>
-      <c r="X15" s="214"/>
+      <c r="S15" s="211"/>
+      <c r="T15" s="211"/>
+      <c r="U15" s="211"/>
+      <c r="V15" s="211"/>
+      <c r="W15" s="211"/>
+      <c r="X15" s="212"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="212" t="s">
+      <c r="B16" s="210" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="213"/>
-      <c r="D16" s="213"/>
-      <c r="E16" s="213"/>
-      <c r="F16" s="213"/>
-      <c r="G16" s="213"/>
-      <c r="H16" s="214"/>
+      <c r="C16" s="211"/>
+      <c r="D16" s="211"/>
+      <c r="E16" s="211"/>
+      <c r="F16" s="211"/>
+      <c r="G16" s="211"/>
+      <c r="H16" s="212"/>
       <c r="J16" s="38" t="s">
         <v>1</v>
       </c>
@@ -11730,24 +11860,24 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
       <c r="H24" s="63"/>
-      <c r="J24" s="212" t="s">
+      <c r="J24" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="K24" s="213"/>
-      <c r="L24" s="213"/>
-      <c r="M24" s="213"/>
-      <c r="N24" s="213"/>
-      <c r="O24" s="213"/>
-      <c r="P24" s="214"/>
-      <c r="R24" s="212" t="s">
+      <c r="K24" s="211"/>
+      <c r="L24" s="211"/>
+      <c r="M24" s="211"/>
+      <c r="N24" s="211"/>
+      <c r="O24" s="211"/>
+      <c r="P24" s="212"/>
+      <c r="R24" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="S24" s="213"/>
-      <c r="T24" s="213"/>
-      <c r="U24" s="213"/>
-      <c r="V24" s="213"/>
-      <c r="W24" s="213"/>
-      <c r="X24" s="214"/>
+      <c r="S24" s="211"/>
+      <c r="T24" s="211"/>
+      <c r="U24" s="211"/>
+      <c r="V24" s="211"/>
+      <c r="W24" s="211"/>
+      <c r="X24" s="212"/>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11"/>
@@ -11797,15 +11927,15 @@
       </c>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="212" t="s">
+      <c r="B26" s="210" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="213"/>
-      <c r="D26" s="213"/>
-      <c r="E26" s="213"/>
-      <c r="F26" s="213"/>
-      <c r="G26" s="213"/>
-      <c r="H26" s="214"/>
+      <c r="C26" s="211"/>
+      <c r="D26" s="211"/>
+      <c r="E26" s="211"/>
+      <c r="F26" s="211"/>
+      <c r="G26" s="211"/>
+      <c r="H26" s="212"/>
       <c r="J26" s="11" t="s">
         <v>114</v>
       </c>
@@ -12298,20 +12428,20 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
-      <c r="J37" s="202" t="s">
+      <c r="J37" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="K37" s="203"/>
-      <c r="L37" s="203"/>
+      <c r="K37" s="225"/>
+      <c r="L37" s="225"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
       <c r="P37" s="9"/>
-      <c r="R37" s="202" t="s">
+      <c r="R37" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="S37" s="203"/>
-      <c r="T37" s="203"/>
+      <c r="S37" s="225"/>
+      <c r="T37" s="225"/>
       <c r="U37" s="8"/>
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
@@ -12385,29 +12515,29 @@
       <c r="X39" s="9"/>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B40" s="202" t="s">
+      <c r="B40" s="224" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="203"/>
-      <c r="D40" s="203"/>
+      <c r="C40" s="225"/>
+      <c r="D40" s="225"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="9"/>
-      <c r="J40" s="202" t="s">
+      <c r="J40" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="K40" s="203"/>
-      <c r="L40" s="203"/>
+      <c r="K40" s="225"/>
+      <c r="L40" s="225"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
       <c r="P40" s="9"/>
-      <c r="R40" s="202" t="s">
+      <c r="R40" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="S40" s="203"/>
-      <c r="T40" s="203"/>
+      <c r="S40" s="225"/>
+      <c r="T40" s="225"/>
       <c r="U40" s="8"/>
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
@@ -12467,11 +12597,11 @@
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B43" s="202" t="s">
+      <c r="B43" s="224" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="203"/>
-      <c r="D43" s="203"/>
+      <c r="C43" s="225"/>
+      <c r="D43" s="225"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
@@ -12503,11 +12633,11 @@
       <c r="H45" s="9"/>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B46" s="202" t="s">
+      <c r="B46" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="C46" s="203"/>
-      <c r="D46" s="203"/>
+      <c r="C46" s="225"/>
+      <c r="D46" s="225"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
@@ -12531,11 +12661,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="R37:T37"/>
-    <mergeCell ref="R40:T40"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="R15:X15"/>
     <mergeCell ref="R24:X24"/>
     <mergeCell ref="J3:P3"/>
@@ -12549,16 +12684,11 @@
     <mergeCell ref="S6:U6"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="W11:X11"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="R37:T37"/>
+    <mergeCell ref="R40:T40"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J40:L40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected Skoll, Added Hati
Corrected improperly indexed fixture values in the Skoll data set. Added
Hati datasets and tracking sheet based on tests conducted on 8/31/2015.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Mass Properties.xlsx
+++ b/Design/CAD/mAEWing1 - Mass Properties.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-255" yWindow="465" windowWidth="25440" windowHeight="14580"/>
+    <workbookView xWindow="-255" yWindow="465" windowWidth="25440" windowHeight="14580" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tracking" sheetId="6" r:id="rId1"/>
-    <sheet name="Test Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="Skoll - Tracking" sheetId="6" r:id="rId1"/>
+    <sheet name="Skoll - Test Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="Hati - Tracking" sheetId="7" r:id="rId3"/>
+    <sheet name="Hati - Test Summary" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="g">'Test Summary'!$K$4</definedName>
-    <definedName name="in2m">'Test Summary'!$K$5</definedName>
+    <definedName name="g">'Skoll - Test Summary'!$K$4</definedName>
+    <definedName name="in2m">'Skoll - Test Summary'!$K$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="72">
   <si>
     <t>Left Wing</t>
   </si>
@@ -221,6 +223,27 @@
   </si>
   <si>
     <t>Repair to Wing Attach</t>
+  </si>
+  <si>
+    <t>Inertia Uncertainty (%)</t>
+  </si>
+  <si>
+    <t>[0]</t>
+  </si>
+  <si>
+    <t>[48.14]</t>
+  </si>
+  <si>
+    <t>[48.21]</t>
+  </si>
+  <si>
+    <t>Airframe (CB2 + WS2)</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -231,7 +254,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +273,13 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -443,10 +473,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -597,9 +628,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -903,9 +947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,31 +1007,31 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <f>'Test Summary'!B19</f>
+        <f>'Skoll - Test Summary'!B19</f>
         <v>6269.81</v>
       </c>
       <c r="D3" s="45">
-        <f>'Test Summary'!C19</f>
-        <v>-23.225000000000001</v>
+        <f>'Skoll - Test Summary'!C19</f>
+        <v>-23.726447721701295</v>
       </c>
       <c r="E3" s="45">
-        <f>'Test Summary'!D19</f>
+        <f>'Skoll - Test Summary'!D19</f>
         <v>0</v>
       </c>
       <c r="F3" s="45">
-        <f>'Test Summary'!E19</f>
-        <v>-0.49249999999999994</v>
+        <f>'Skoll - Test Summary'!E19</f>
+        <v>-0.49104200924748914</v>
       </c>
       <c r="G3" s="46">
-        <f>'Test Summary'!F19</f>
+        <f>'Skoll - Test Summary'!F19</f>
         <v>3.0977856600061244</v>
       </c>
       <c r="H3" s="46">
-        <f>'Test Summary'!G19</f>
-        <v>0.46361697672372681</v>
+        <f>'Skoll - Test Summary'!G19</f>
+        <v>0.5278392103037457</v>
       </c>
       <c r="I3" s="46">
-        <f>'Test Summary'!H19</f>
+        <f>'Skoll - Test Summary'!H19</f>
         <v>3.3146271438643926</v>
       </c>
       <c r="J3" t="s">
@@ -1006,15 +1050,15 @@
         <v>-109.34</v>
       </c>
       <c r="D5" s="45">
-        <f>'Test Summary'!C8</f>
+        <f>'Skoll - Test Summary'!C8</f>
         <v>-4.62</v>
       </c>
       <c r="E5" s="45">
-        <f>'Test Summary'!D8</f>
+        <f>'Skoll - Test Summary'!D8</f>
         <v>0</v>
       </c>
       <c r="F5" s="45">
-        <f>'Test Summary'!E8</f>
+        <f>'Skoll - Test Summary'!E8</f>
         <v>-0.9</v>
       </c>
       <c r="G5" s="48">
@@ -1041,7 +1085,7 @@
       </c>
       <c r="D6" s="45">
         <f>(D3*$C3 + D5*$C5)/$C6</f>
-        <v>-23.555213555134593</v>
+        <v>-24.065561294836272</v>
       </c>
       <c r="E6" s="45">
         <f t="shared" ref="E6:F6" si="0">(E3*$C3 + E5*$C5)/$C6</f>
@@ -1049,19 +1093,19 @@
       </c>
       <c r="F6" s="45">
         <f t="shared" si="0"/>
-        <v>-0.48526742683593937</v>
+        <v>-0.48378355872198059</v>
       </c>
       <c r="G6" s="46">
         <f>(G3+($C3/1000)*(($E3*in2m-$E6*in2m)^2+($F3*in2m-$F6*in2m)^2)) + SIGN($C5)*((G5)+ABS($C5/1000)*(($E5*in2m-$E6*in2m)^2+($F5*in2m-$F6*in2m)^2))</f>
-        <v>3.0977737381943125</v>
+        <v>3.0977736527318012</v>
       </c>
       <c r="H6" s="46">
         <f>(H3+($C3/1000)*(($D3*in2m-$D6*in2m)^2+($F3*in2m-$F6*in2m)^2)) + SIGN($C5)*((H5)+ABS($C5/1000)*(($D5*in2m-$D6*in2m)^2+($F5*in2m-$F6*in2m)^2))</f>
-        <v>0.43875391097981603</v>
+        <v>0.50161841510085492</v>
       </c>
       <c r="I6" s="46">
         <f>(I3+($C3/1000)*(($D3*in2m-$D6*in2m)^2+($E3*in2m-$E6*in2m)^2)) + SIGN($C5)*((I5)+ABS($C5/1000)*(($D5*in2m-$D6*in2m)^2+($E5*in2m-$E6*in2m)^2))</f>
-        <v>3.289775999932294</v>
+        <v>3.2884183559358253</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1081,27 +1125,27 @@
         <v>-104.4</v>
       </c>
       <c r="D8" s="45">
-        <f>'Test Summary'!C7</f>
+        <f>'Skoll - Test Summary'!C7</f>
         <v>-9.0909999999999993</v>
       </c>
       <c r="E8" s="45">
-        <f>'Test Summary'!D7</f>
+        <f>'Skoll - Test Summary'!D7</f>
         <v>0</v>
       </c>
       <c r="F8" s="45">
-        <f>'Test Summary'!E7</f>
+        <f>'Skoll - Test Summary'!E7</f>
         <v>-1.9730000000000001</v>
       </c>
       <c r="G8" s="48">
-        <f>'Test Summary'!F7</f>
+        <f>'Skoll - Test Summary'!F7</f>
         <v>3.1799999999999998E-4</v>
       </c>
       <c r="H8" s="48">
-        <f>'Test Summary'!G7</f>
+        <f>'Skoll - Test Summary'!G7</f>
         <v>5.9639999999999997E-4</v>
       </c>
       <c r="I8" s="48">
-        <f>'Test Summary'!H7</f>
+        <f>'Skoll - Test Summary'!H7</f>
         <v>8.8159999999999996E-4</v>
       </c>
     </row>
@@ -1116,7 +1160,7 @@
       </c>
       <c r="D9" s="45">
         <f>(D6*$C6 + D8*$C8)/$C9</f>
-        <v>-23.804560721722172</v>
+        <v>-24.323706296327487</v>
       </c>
       <c r="E9" s="45">
         <f t="shared" ref="E9" si="1">(E6*$C6 + E8*$C8)/$C9</f>
@@ -1124,19 +1168,19 @@
       </c>
       <c r="F9" s="45">
         <f t="shared" ref="F9" si="2">(F6*$C6 + F8*$C8)/$C9</f>
-        <v>-0.45962055012574149</v>
+        <v>-0.4581111017541078</v>
       </c>
       <c r="G9" s="46">
         <f>(G6+($C6/1000)*(($E6*in2m-$E9*in2m)^2+($F6*in2m-$F9*in2m)^2)) + SIGN($C8)*((G8)+ABS($C8/1000)*(($E8*in2m-$E9*in2m)^2+($F8*in2m-$F9*in2m)^2))</f>
-        <v>3.097304088815362</v>
+        <v>3.0973037006910635</v>
       </c>
       <c r="H9" s="46">
         <f>(H6+($C6/1000)*(($D6*in2m-$D9*in2m)^2+($F6*in2m-$F9*in2m)^2)) + SIGN($C8)*((H8)+ABS($C8/1000)*(($D8*in2m-$D9*in2m)^2+($F8*in2m-$F9*in2m)^2))</f>
-        <v>0.42367142780846218</v>
+        <v>0.48550624667414077</v>
       </c>
       <c r="I9" s="46">
         <f>(I6+($C6/1000)*(($D6*in2m-$D9*in2m)^2+($E6*in2m-$E9*in2m)^2)) + SIGN($C8)*((I8)+ABS($C8/1000)*(($D8*in2m-$D9*in2m)^2+($E8*in2m-$E9*in2m)^2))</f>
-        <v>3.2745599661398908</v>
+        <v>3.2721729395498484</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1190,7 +1234,7 @@
       </c>
       <c r="D12" s="45">
         <f>(D9*$C9 + D11*$C11)/$C12</f>
-        <v>-23.882999220064654</v>
+        <v>-24.398146832659627</v>
       </c>
       <c r="E12" s="45">
         <f t="shared" ref="E12" si="3">(E9*$C9 + E11*$C11)/$C12</f>
@@ -1198,19 +1242,19 @@
       </c>
       <c r="F12" s="45">
         <f t="shared" ref="F12" si="4">(F9*$C9 + F11*$C11)/$C12</f>
-        <v>-0.46563028524988231</v>
+        <v>-0.46413246120395141</v>
       </c>
       <c r="G12" s="46">
         <f>(G9+($C9/1000)*(($E9*in2m-$E12*in2m)^2+($F9*in2m-$F12*in2m)^2)) + SIGN($C11)*((G11)+ABS($C11/1000)*(($E11*in2m-$E12*in2m)^2+($F11*in2m-$F12*in2m)^2))</f>
-        <v>3.0973224127812715</v>
+        <v>3.0973220956117635</v>
       </c>
       <c r="H12" s="46">
         <f>(H9+($C9/1000)*(($D9*in2m-$D12*in2m)^2+($F9*in2m-$F12*in2m)^2)) + SIGN($C11)*((H11)+ABS($C11/1000)*(($D11*in2m-$D12*in2m)^2+($F11*in2m-$F12*in2m)^2))</f>
-        <v>0.42681128063342277</v>
+        <v>0.48833607499407028</v>
       </c>
       <c r="I12" s="46">
         <f>(I9+($C9/1000)*(($D9*in2m-$D12*in2m)^2+($E9*in2m-$E12*in2m)^2)) + SIGN($C11)*((I11)+ABS($C11/1000)*(($D11*in2m-$D12*in2m)^2+($E11*in2m-$E12*in2m)^2))</f>
-        <v>3.2776814949989417</v>
+        <v>3.2749843729490777</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1268,7 +1312,7 @@
       </c>
       <c r="D15" s="45">
         <f>(D12*$C12 + D14*$C14)/$C15</f>
-        <v>-23.74374809083487</v>
+        <v>-24.254046129974174</v>
       </c>
       <c r="E15" s="45">
         <f t="shared" ref="E15" si="5">(E12*$C12 + E14*$C14)/$C15</f>
@@ -1276,19 +1320,19 @@
       </c>
       <c r="F15" s="45">
         <f t="shared" ref="F15" si="6">(F12*$C12 + F14*$C14)/$C15</f>
-        <v>-0.47982058717073489</v>
+        <v>-0.47833686356428345</v>
       </c>
       <c r="G15" s="46">
         <f>(G12+($C12/1000)*(($E12*in2m-$E15*in2m)^2+($F12*in2m-$F15*in2m)^2)) + SIGN($C14)*((G14)+ABS($C14/1000)*(($E14*in2m-$E15*in2m)^2+($F14*in2m-$F15*in2m)^2))</f>
-        <v>3.0975833017689669</v>
+        <v>3.0975831520605559</v>
       </c>
       <c r="H15" s="46">
         <f>(H12+($C12/1000)*(($D12*in2m-$D15*in2m)^2+($F12*in2m-$F15*in2m)^2)) + SIGN($C14)*((H14)+ABS($C14/1000)*(($D14*in2m-$D15*in2m)^2+($F14*in2m-$F15*in2m)^2))</f>
-        <v>0.43533721969487132</v>
+        <v>0.49743692426532682</v>
       </c>
       <c r="I15" s="46">
         <f>(I12+($C12/1000)*(($D12*in2m-$D15*in2m)^2+($E12*in2m-$E15*in2m)^2)) + SIGN($C14)*((I14)+ABS($C14/1000)*(($D14*in2m-$D15*in2m)^2+($E14*in2m-$E15*in2m)^2))</f>
-        <v>3.2862816561838057</v>
+        <v>3.2841592768826526</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1339,7 +1383,7 @@
       </c>
       <c r="D18" s="45">
         <f>(D15*$C15 + D17*$C17)/$C18</f>
-        <v>-23.244952087156793</v>
+        <v>-23.741940255166316</v>
       </c>
       <c r="E18" s="45">
         <f t="shared" ref="E18" si="8">(E15*$C15 + E17*$C17)/$C18</f>
@@ -1347,19 +1391,19 @@
       </c>
       <c r="F18" s="45">
         <f t="shared" ref="F18" si="9">(F15*$C15 + F17*$C17)/$C18</f>
-        <v>-0.49077993525206004</v>
+        <v>-0.48933491093206366</v>
       </c>
       <c r="G18" s="46">
         <f>(G15+($C15/1000)*(($E15*in2m-$E18*in2m)^2+($F15*in2m-$F18*in2m)^2)) + SIGN($C17)*((G17)+ABS($C17/1000)*(($E17*in2m-$E18*in2m)^2+($F17*in2m-$F18*in2m)^2))</f>
-        <v>3.0976016056450537</v>
+        <v>3.0976015854329564</v>
       </c>
       <c r="H18" s="46">
         <f>(H15+($C15/1000)*(($D15*in2m-$D18*in2m)^2+($F15*in2m-$F18*in2m)^2)) + SIGN($C17)*((H17)+ABS($C17/1000)*(($D17*in2m-$D18*in2m)^2+($F17*in2m-$F18*in2m)^2))</f>
-        <v>0.47327126526614754</v>
+        <v>0.53742158377972804</v>
       </c>
       <c r="I18" s="46">
         <f>(I15+($C15/1000)*(($D15*in2m-$D18*in2m)^2+($E15*in2m-$E18*in2m)^2)) + SIGN($C17)*((I17)+ABS($C17/1000)*(($D17*in2m-$D18*in2m)^2+($E17*in2m-$E18*in2m)^2))</f>
-        <v>3.3241973978789954</v>
+        <v>3.3241255030246535</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1404,7 +1448,7 @@
       </c>
       <c r="D21" s="45">
         <f>(D18*$C18 + D20*$C20)/$C21</f>
-        <v>-23.381373435366637</v>
+        <v>-23.89546138022941</v>
       </c>
       <c r="E21" s="45">
         <f t="shared" ref="E21:F21" si="10">(E18*$C18 + E20*$C20)/$C21</f>
@@ -1412,19 +1456,19 @@
       </c>
       <c r="F21" s="45">
         <f t="shared" si="10"/>
-        <v>-0.47838591237235611</v>
+        <v>-0.47689116937692644</v>
       </c>
       <c r="G21" s="46">
         <f>(G18+($C18/1000)*(($E18*in2m-$E21*in2m)^2+($F18*in2m-$F21*in2m)^2)) + SIGN($C20)*((G20)+ABS($C20/1000)*(($E20*in2m-$E21*in2m)^2+($F20*in2m-$F21*in2m)^2))</f>
-        <v>3.0975833842501732</v>
+        <v>3.097583217554448</v>
       </c>
       <c r="H21" s="46">
         <f>(H18+($C18/1000)*(($D18*in2m-$D21*in2m)^2+($F18*in2m-$F21*in2m)^2)) + SIGN($C20)*((H20)+ABS($C20/1000)*(($D20*in2m-$D21*in2m)^2+($F20*in2m-$F21*in2m)^2))</f>
-        <v>0.47104543715176045</v>
+        <v>0.53460749816464148</v>
       </c>
       <c r="I21" s="46">
         <f>(I18+($C18/1000)*(($D18*in2m-$D21*in2m)^2+($E18*in2m-$E21*in2m)^2)) + SIGN($C20)*((I20)+ABS($C20/1000)*(($D20*in2m-$D21*in2m)^2+($E20*in2m-$E21*in2m)^2))</f>
-        <v>3.3219897911594889</v>
+        <v>3.3213297852880754</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1472,7 +1516,7 @@
       </c>
       <c r="D24" s="45">
         <f>(D21*$C21 + D23*$C23)/$C24</f>
-        <v>-23.044856295658093</v>
+        <v>-23.516763393667937</v>
       </c>
       <c r="E24" s="45">
         <f t="shared" ref="E24:F24" si="11">(E21*$C21 + E23*$C23)/$C24</f>
@@ -1480,19 +1524,19 @@
       </c>
       <c r="F24" s="45">
         <f t="shared" si="11"/>
-        <v>-0.50895884823386539</v>
+        <v>-0.50758674870052189</v>
       </c>
       <c r="G24" s="46">
         <f>(G21+($C21/1000)*(($E21*in2m-$E24*in2m)^2+($F21*in2m-$F24*in2m)^2)) + SIGN($C23)*((G23)+ABS($C23/1000)*(($E23*in2m-$E24*in2m)^2+($F23*in2m-$F24*in2m)^2))</f>
-        <v>3.0976283318464786</v>
+        <v>3.0976285264890047</v>
       </c>
       <c r="H24" s="46">
         <f>(H21+($C21/1000)*(($D21*in2m-$D24*in2m)^2+($F21*in2m-$F24*in2m)^2)) + SIGN($C23)*((H23)+ABS($C23/1000)*(($D23*in2m-$D24*in2m)^2+($F23*in2m-$F24*in2m)^2))</f>
-        <v>0.47653599504731975</v>
+        <v>0.54154913929713655</v>
       </c>
       <c r="I24" s="46">
         <f>(I21+($C21/1000)*(($D21*in2m-$D24*in2m)^2+($E21*in2m-$E24*in2m)^2)) + SIGN($C23)*((I23)+ABS($C23/1000)*(($D23*in2m-$D24*in2m)^2+($E23*in2m-$E24*in2m)^2))</f>
-        <v>3.3274354014587431</v>
+        <v>3.3282261174860137</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1543,7 +1587,7 @@
       </c>
       <c r="D27" s="45">
         <f>(D24*$C24 + D26*$C26)/$C27</f>
-        <v>-23.512759265786194</v>
+        <v>-23.996650540456095</v>
       </c>
       <c r="E27" s="45">
         <f t="shared" ref="E27:F27" si="13">(E24*$C24 + E26*$C26)/$C27</f>
@@ -1551,19 +1595,19 @@
       </c>
       <c r="F27" s="45">
         <f t="shared" si="13"/>
-        <v>-0.49902827871312483</v>
+        <v>-0.49762133443327916</v>
       </c>
       <c r="G27" s="46">
         <f>(G24+($C24/1000)*(($E24*in2m-$E27*in2m)^2+($F24*in2m-$F27*in2m)^2)) + SIGN($C26)*((G26)+ABS($C26/1000)*(($E26*in2m-$E27*in2m)^2+($F26*in2m-$F27*in2m)^2))</f>
-        <v>3.0976116406455296</v>
+        <v>3.0976117179491589</v>
       </c>
       <c r="H27" s="46">
         <f>(H24+($C24/1000)*(($D24*in2m-$D27*in2m)^2+($F24*in2m-$F27*in2m)^2)) + SIGN($C26)*((H26)+ABS($C26/1000)*(($D26*in2m-$D27*in2m)^2+($F26*in2m-$F27*in2m)^2))</f>
-        <v>0.43946395744586064</v>
+        <v>0.50255451400140949</v>
       </c>
       <c r="I27" s="46">
         <f>(I24+($C24/1000)*(($D24*in2m-$D27*in2m)^2+($E24*in2m-$E27*in2m)^2)) + SIGN($C26)*((I26)+ABS($C26/1000)*(($D26*in2m-$D27*in2m)^2+($E26*in2m-$E27*in2m)^2))</f>
-        <v>3.2903800550582329</v>
+        <v>3.2892483007301321</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1611,7 +1655,7 @@
       </c>
       <c r="D30" s="45">
         <f>(D27*$C27 + D29*$C29)/$C30</f>
-        <v>-23.589704227844443</v>
+        <v>-24.077726645338842</v>
       </c>
       <c r="E30" s="45">
         <f t="shared" ref="E30:F30" si="15">(E27*$C27 + E29*$C29)/$C30</f>
@@ -1619,19 +1663,19 @@
       </c>
       <c r="F30" s="45">
         <f t="shared" si="15"/>
-        <v>-0.49048264592249013</v>
+        <v>-0.48906369008535788</v>
       </c>
       <c r="G30" s="46">
         <f>(G27+($C27/1000)*(($E27*in2m-$E30*in2m)^2+($F27*in2m-$F30*in2m)^2)) + SIGN($C29)*((G29)+ABS($C29/1000)*(($E29*in2m-$E30*in2m)^2+($F29*in2m-$F30*in2m)^2))</f>
-        <v>3.0974952641665183</v>
+        <v>3.0974952406015652</v>
       </c>
       <c r="H30" s="46">
         <f>(H27+($C27/1000)*(($D27*in2m-$D30*in2m)^2+($F27*in2m-$F30*in2m)^2)) + SIGN($C29)*((H29)+ABS($C29/1000)*(($D29*in2m-$D30*in2m)^2+($F29*in2m-$F30*in2m)^2))</f>
-        <v>0.43652115056506763</v>
+        <v>0.4992910808410852</v>
       </c>
       <c r="I30" s="46">
         <f>(I27+($C27/1000)*(($D27*in2m-$D30*in2m)^2+($E27*in2m-$E30*in2m)^2)) + SIGN($C29)*((I29)+ABS($C29/1000)*(($D29*in2m-$D30*in2m)^2+($E29*in2m-$E30*in2m)^2))</f>
-        <v>3.2873925843392571</v>
+        <v>3.2859403046002069</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1679,7 +1723,7 @@
       </c>
       <c r="D33" s="45">
         <f>(D30*$C30 + D32*$C32)/$C33</f>
-        <v>-23.580479807735223</v>
+        <v>-24.06437108240512</v>
       </c>
       <c r="E33" s="45">
         <f t="shared" ref="E33:F33" si="17">(E30*$C30 + E32*$C32)/$C33</f>
@@ -1687,19 +1731,19 @@
       </c>
       <c r="F33" s="45">
         <f t="shared" si="17"/>
-        <v>-0.49691201177721772</v>
+        <v>-0.495505067497372</v>
       </c>
       <c r="G33" s="46">
         <f>(G30+($C30/1000)*(($E30*in2m-$E33*in2m)^2+($F30*in2m-$F33*in2m)^2)) + SIGN($C32)*((G32)+ABS($C32/1000)*(($E32*in2m-$E33*in2m)^2+($F32*in2m-$F33*in2m)^2))</f>
-        <v>3.0985848209052169</v>
+        <v>3.0985848732469812</v>
       </c>
       <c r="H33" s="46">
         <f>(H30+($C30/1000)*(($D30*in2m-$D33*in2m)^2+($F30*in2m-$F33*in2m)^2)) + SIGN($C32)*((H32)+ABS($C32/1000)*(($D32*in2m-$D33*in2m)^2+($F32*in2m-$F33*in2m)^2))</f>
-        <v>0.43658322545678441</v>
+        <v>0.49939903223107446</v>
       </c>
       <c r="I33" s="46">
         <f>(I30+($C30/1000)*(($D30*in2m-$D33*in2m)^2+($E30*in2m-$E33*in2m)^2)) + SIGN($C32)*((I32)+ABS($C32/1000)*(($D32*in2m-$D33*in2m)^2+($E32*in2m-$E33*in2m)^2))</f>
-        <v>3.2885036236808043</v>
+        <v>3.287097144533309</v>
       </c>
       <c r="J33" t="s">
         <v>14</v>
@@ -1747,7 +1791,7 @@
       </c>
       <c r="D36" s="45">
         <f>(D33*$C33 + D35*$C35)/$C36</f>
-        <v>-23.564105221230982</v>
+        <v>-24.042983132555808</v>
       </c>
       <c r="E36" s="45">
         <f t="shared" ref="E36:F36" si="18">(E33*$C33 + E35*$C35)/$C36</f>
@@ -1755,19 +1799,19 @@
       </c>
       <c r="F36" s="45">
         <f t="shared" si="18"/>
-        <v>-0.49176374687562335</v>
+        <v>-0.49037137926465013</v>
       </c>
       <c r="G36" s="46">
         <f>(G33+($C33/1000)*(($E33*in2m-$E36*in2m)^2+($F33*in2m-$F36*in2m)^2)) + SIGN($C35)*((G35)+ABS($C35/1000)*(($E35*in2m-$E36*in2m)^2+($F35*in2m-$F36*in2m)^2))</f>
-        <v>3.0985955942841277</v>
+        <v>3.0985955859868679</v>
       </c>
       <c r="H36" s="46">
         <f>(H33+($C33/1000)*(($D33*in2m-$D36*in2m)^2+($F33*in2m-$F36*in2m)^2)) + SIGN($C35)*((H35)+ABS($C35/1000)*(($D35*in2m-$D36*in2m)^2+($F35*in2m-$F36*in2m)^2))</f>
-        <v>0.43670243136687792</v>
+        <v>0.49959477395043728</v>
       </c>
       <c r="I36" s="46">
         <f>(I33+($C33/1000)*(($D33*in2m-$D36*in2m)^2+($E33*in2m-$E36*in2m)^2)) + SIGN($C35)*((I35)+ABS($C35/1000)*(($D35*in2m-$D36*in2m)^2+($E35*in2m-$E36*in2m)^2))</f>
-        <v>3.2886121557965287</v>
+        <v>3.2872822730973268</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1812,7 +1856,7 @@
       </c>
       <c r="D39" s="45">
         <f>(D36*$C36 + D38*$C38)/$C39</f>
-        <v>-23.225314613918609</v>
+        <v>-23.695628418545784</v>
       </c>
       <c r="E39" s="45">
         <f t="shared" ref="E39:F39" si="19">(E36*$C36 + E38*$C38)/$C39</f>
@@ -1820,19 +1864,19 @@
       </c>
       <c r="F39" s="45">
         <f t="shared" si="19"/>
-        <v>-0.49906451967580451</v>
+        <v>-0.49769705274306414</v>
       </c>
       <c r="G39" s="46">
         <f>(G36+($C36/1000)*(($E36*in2m-$E39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((G38)+ABS($C38/1000)*(($E38*in2m-$E39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
-        <v>3.0986083035190108</v>
+        <v>3.0986083814829324</v>
       </c>
       <c r="H39" s="46">
         <f>(H36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((H38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
-        <v>0.46389997992190185</v>
+        <v>0.52818416630470488</v>
       </c>
       <c r="I39" s="46">
         <f>(I36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($E36*in2m-$E39*in2m)^2)) + SIGN($C38)*((I38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($E38*in2m-$E39*in2m)^2))</f>
-        <v>3.3157971652325342</v>
+        <v>3.3158590400713943</v>
       </c>
       <c r="J39" t="s">
         <v>55</v>
@@ -1887,7 +1931,7 @@
       </c>
       <c r="D42" s="45">
         <f>(D39*$C39 + D41*$C41)/$C42</f>
-        <v>-23.231331679703636</v>
+        <v>-23.705547114117035</v>
       </c>
       <c r="E42" s="45">
         <f t="shared" ref="E42:F42" si="21">(E39*$C39 + E41*$C41)/$C42</f>
@@ -1895,19 +1939,19 @@
       </c>
       <c r="F42" s="45">
         <f t="shared" si="21"/>
-        <v>-0.49283490827860593</v>
+        <v>-0.49145609711215615</v>
       </c>
       <c r="G42" s="46">
         <f>(G39+($C39/1000)*(($E39*in2m-$E42*in2m)^2+($F39*in2m-$F42*in2m)^2)) + SIGN($C41)*((G41)+ABS($C41/1000)*(($E41*in2m-$E42*in2m)^2+($F41*in2m-$F42*in2m)^2))</f>
-        <v>3.0975187519037584</v>
+        <v>3.0975187563210489</v>
       </c>
       <c r="H42" s="46">
         <f>(H39+($C39/1000)*(($D39*in2m-$D42*in2m)^2+($F39*in2m-$F42*in2m)^2)) + SIGN($C41)*((H41)+ABS($C41/1000)*(($D41*in2m-$D42*in2m)^2+($F41*in2m-$F42*in2m)^2))</f>
-        <v>0.46386098224327083</v>
+        <v>0.52811277143705515</v>
       </c>
       <c r="I42" s="46">
         <f>(I39+($C39/1000)*(($D39*in2m-$D42*in2m)^2+($E39*in2m-$E42*in2m)^2)) + SIGN($C41)*((I41)+ABS($C41/1000)*(($D41*in2m-$D42*in2m)^2+($E41*in2m-$E42*in2m)^2))</f>
-        <v>3.3147089668479501</v>
+        <v>3.3147385180444222</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1954,7 +1998,7 @@
       </c>
       <c r="D45" s="45">
         <f>(D42*$C42 + D44*$C44)/$C45</f>
-        <v>-23.051326767134604</v>
+        <v>-23.518773597725787</v>
       </c>
       <c r="E45" s="45">
         <f t="shared" ref="E45:F45" si="22">(E42*$C42 + E44*$C44)/$C45</f>
@@ -1962,19 +2006,19 @@
       </c>
       <c r="F45" s="45">
         <f t="shared" si="22"/>
-        <v>-0.49864648461311989</v>
+        <v>-0.49728735358749659</v>
       </c>
       <c r="G45" s="46">
         <f>(G42+($C42/1000)*(($E42*in2m-$E45*in2m)^2+($F42*in2m-$F45*in2m)^2)) + SIGN($C44)*((G44)+ABS($C44/1000)*(($E44*in2m-$E45*in2m)^2+($F44*in2m-$F45*in2m)^2))</f>
-        <v>3.0975288826567486</v>
+        <v>3.0975289557390107</v>
       </c>
       <c r="H45" s="46">
         <f>(H42+($C42/1000)*(($D42*in2m-$D45*in2m)^2+($F42*in2m-$F45*in2m)^2)) + SIGN($C44)*((H44)+ABS($C44/1000)*(($D44*in2m-$D45*in2m)^2+($F44*in2m-$F45*in2m)^2))</f>
-        <v>0.47358105584380839</v>
+        <v>0.5385768765737533</v>
       </c>
       <c r="I45" s="46">
         <f>(I42+($C42/1000)*(($D42*in2m-$D45*in2m)^2+($E42*in2m-$E45*in2m)^2)) + SIGN($C44)*((I44)+ABS($C44/1000)*(($D44*in2m-$D45*in2m)^2+($E44*in2m-$E45*in2m)^2))</f>
-        <v>3.3244189286025736</v>
+        <v>3.3251924426702351</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2020,7 +2064,7 @@
       </c>
       <c r="D48" s="45">
         <f>(D45*$C45 + D47*$C47)/$C48</f>
-        <v>-23.250768223256866</v>
+        <v>-23.723273196310103</v>
       </c>
       <c r="E48" s="45">
         <f t="shared" ref="E48:F48" si="23">(E45*$C45 + E47*$C47)/$C48</f>
@@ -2028,19 +2072,19 @@
       </c>
       <c r="F48" s="45">
         <f t="shared" si="23"/>
-        <v>-0.49430352381925652</v>
+        <v>-0.49292968592666508</v>
       </c>
       <c r="G48" s="46">
         <f>(G45+($C45/1000)*(($E45*in2m-$E48*in2m)^2+($F45*in2m-$F48*in2m)^2)) + SIGN($C47)*((G47)+ABS($C47/1000)*(($E47*in2m-$E48*in2m)^2+($F47*in2m-$F48*in2m)^2))</f>
-        <v>3.0975213119976854</v>
+        <v>3.0975213337669709</v>
       </c>
       <c r="H48" s="46">
         <f>(H45+($C45/1000)*(($D45*in2m-$D48*in2m)^2+($F45*in2m-$F48*in2m)^2)) + SIGN($C47)*((H47)+ABS($C47/1000)*(($D47*in2m-$D48*in2m)^2+($F47*in2m-$F48*in2m)^2))</f>
-        <v>0.45762251515309599</v>
+        <v>0.52179894209209343</v>
       </c>
       <c r="I48" s="46">
         <f>(I45+($C45/1000)*(($D45*in2m-$D48*in2m)^2+($E45*in2m-$E48*in2m)^2)) + SIGN($C47)*((I47)+ABS($C47/1000)*(($D47*in2m-$D48*in2m)^2+($E47*in2m-$E48*in2m)^2))</f>
-        <v>3.3084679444417651</v>
+        <v>3.3084221160314553</v>
       </c>
       <c r="J48" t="s">
         <v>55</v>
@@ -2090,7 +2134,7 @@
       </c>
       <c r="D51" s="45">
         <f>(D48*$C48 + D50*$C50)/$C51</f>
-        <v>-23.291099104253739</v>
+        <v>-23.760780564577079</v>
       </c>
       <c r="E51" s="45">
         <f t="shared" ref="E51:F51" si="24">(E48*$C48 + E50*$C50)/$C51</f>
@@ -2098,19 +2142,19 @@
       </c>
       <c r="F51" s="45">
         <f t="shared" si="24"/>
-        <v>-0.49134975111520085</v>
+        <v>-0.48998412276324865</v>
       </c>
       <c r="G51" s="46">
         <f>(G48+($C48/1000)*(($E48*in2m-$E51*in2m)^2+($F48*in2m-$F51*in2m)^2)) + SIGN($C50)*((G50)+ABS($C50/1000)*(($E50*in2m-$E51*in2m)^2+($F50*in2m-$F51*in2m)^2))</f>
-        <v>3.0975275836941862</v>
+        <v>3.0975275706714465</v>
       </c>
       <c r="H51" s="46">
         <f>(H48+($C48/1000)*(($D48*in2m-$D51*in2m)^2+($F48*in2m-$F51*in2m)^2)) + SIGN($C50)*((H50)+ABS($C50/1000)*(($D50*in2m-$D51*in2m)^2+($F50*in2m-$F51*in2m)^2))</f>
-        <v>0.45879729481710602</v>
+        <v>0.52281580208634781</v>
       </c>
       <c r="I51" s="46">
         <f>(I48+($C48/1000)*(($D48*in2m-$D51*in2m)^2+($E48*in2m-$E51*in2m)^2)) + SIGN($C50)*((I50)+ABS($C50/1000)*(($D50*in2m-$D51*in2m)^2+($E50*in2m-$E51*in2m)^2))</f>
-        <v>3.3096364602963324</v>
+        <v>3.3094327470082918</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2155,7 +2199,7 @@
       </c>
       <c r="D54" s="45">
         <f>(D51*$C51 + D53*$C53)/$C54</f>
-        <v>-23.249353340209801</v>
+        <v>-23.717984663564291</v>
       </c>
       <c r="E54" s="45">
         <f t="shared" ref="E54:F54" si="25">(E51*$C51 + E53*$C53)/$C54</f>
@@ -2163,19 +2207,19 @@
       </c>
       <c r="F54" s="45">
         <f t="shared" si="25"/>
-        <v>-0.49226343149208635</v>
+        <v>-0.49090085647934217</v>
       </c>
       <c r="G54" s="46">
         <f>(G51+($C51/1000)*(($E51*in2m-$E54*in2m)^2+($F51*in2m-$F54*in2m)^2)) + SIGN($C53)*((G53)+ABS($C53/1000)*(($E53*in2m-$E54*in2m)^2+($F53*in2m-$F54*in2m)^2))</f>
-        <v>3.0975291976252439</v>
+        <v>3.0975291953975854</v>
       </c>
       <c r="H54" s="46">
         <f>(H51+($C51/1000)*(($D51*in2m-$D54*in2m)^2+($F51*in2m-$F54*in2m)^2)) + SIGN($C53)*((H53)+ABS($C53/1000)*(($D53*in2m-$D54*in2m)^2+($F53*in2m-$F54*in2m)^2))</f>
-        <v>0.46216500218600121</v>
+        <v>0.52635500214485431</v>
       </c>
       <c r="I54" s="46">
         <f>(I51+($C51/1000)*(($D51*in2m-$D54*in2m)^2+($E51*in2m-$E54*in2m)^2)) + SIGN($C53)*((I53)+ABS($C53/1000)*(($D53*in2m-$D54*in2m)^2+($E53*in2m-$E54*in2m)^2))</f>
-        <v>3.3130025566675698</v>
+        <v>3.3129703252740588</v>
       </c>
       <c r="J54" t="s">
         <v>55</v>
@@ -2210,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,19 +2335,19 @@
         <v>3169.45</v>
       </c>
       <c r="C6" s="23">
-        <v>-18.55</v>
+        <v>-18.523510031077947</v>
       </c>
       <c r="D6" s="24">
         <v>0</v>
       </c>
       <c r="E6" s="25">
-        <v>0.29000000000000004</v>
+        <v>-0.42442166874378823</v>
       </c>
       <c r="F6" s="26">
         <v>1.5280065868500196E-2</v>
       </c>
       <c r="G6" s="26">
-        <v>0.13457839359793833</v>
+        <v>0.14448048825940063</v>
       </c>
       <c r="H6" s="27" t="s">
         <v>37</v>
@@ -2407,9 +2451,15 @@
       <c r="B11" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
+      <c r="C11" s="29">
+        <v>-28.06</v>
+      </c>
+      <c r="D11" s="30">
+        <v>-7.5209999999999999</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0.14099999999999999</v>
+      </c>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
       <c r="H11" s="54"/>
@@ -2421,9 +2471,15 @@
       <c r="B12" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
+      <c r="C12" s="29">
+        <v>-28.06</v>
+      </c>
+      <c r="D12" s="30">
+        <v>7.5209999999999999</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0.14099999999999999</v>
+      </c>
       <c r="F12" s="53"/>
       <c r="G12" s="53"/>
       <c r="H12" s="54"/>
@@ -2442,7 +2498,7 @@
         <v>-31.416080260883309</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
@@ -2462,7 +2518,7 @@
         <v>31.763774206345854</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
@@ -2543,23 +2599,22 @@
         <v>34</v>
       </c>
       <c r="B19" s="34">
-        <f>SUM(B6:B18)</f>
         <v>6269.81</v>
       </c>
       <c r="C19" s="35">
-        <v>-23.225000000000001</v>
+        <v>-23.726447721701295</v>
       </c>
       <c r="D19" s="36">
         <v>0</v>
       </c>
       <c r="E19" s="37">
-        <v>-0.49249999999999994</v>
+        <v>-0.49104200924748914</v>
       </c>
       <c r="F19" s="38">
         <v>3.0977856600061244</v>
       </c>
       <c r="G19" s="38">
-        <v>0.46361697672372681</v>
+        <v>0.5278392103037457</v>
       </c>
       <c r="H19" s="39">
         <v>3.3146271438643926</v>
@@ -2582,7 +2637,7 @@
       </c>
       <c r="G21" s="41">
         <f>G19*$K$6</f>
-        <v>1584.2589043929354</v>
+        <v>1803.7173162227903</v>
       </c>
       <c r="H21" s="42">
         <f>H19*$K$6</f>
@@ -2655,49 +2710,49 @@
       <c r="B27" s="55">
         <v>3529.28</v>
       </c>
-      <c r="C27" s="23">
-        <v>-18.55</v>
+      <c r="C27" s="24">
+        <f>C6</f>
+        <v>-18.523510031077947</v>
       </c>
       <c r="D27" s="24">
+        <f t="shared" ref="D27:E27" si="0">D6</f>
         <v>0</v>
       </c>
       <c r="E27" s="25">
-        <v>0.29000000000000004</v>
-      </c>
-      <c r="F27" s="26">
-        <v>1.5280065868500196E-2</v>
-      </c>
-      <c r="G27" s="26">
-        <v>0.13457839359793833</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>37</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>-0.42442166874378823</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="30">
+        <f t="shared" ref="C28:E38" si="1">C7</f>
         <v>-9.0909999999999993</v>
       </c>
       <c r="D28" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28" s="31">
+        <f t="shared" si="1"/>
         <v>-1.9730000000000001</v>
       </c>
       <c r="F28" s="53">
-        <v>1.7666666666666666E-4</v>
+        <v>1.7896479999999999E-4</v>
       </c>
       <c r="G28" s="53">
-        <v>3.3133333333333333E-4</v>
+        <v>3.3355800000000002E-4</v>
       </c>
       <c r="H28" s="54">
-        <v>4.8977777777777778E-4</v>
+        <v>4.939454E-4</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2707,13 +2762,16 @@
       <c r="B29" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="30">
+        <f t="shared" si="1"/>
         <v>-4.62</v>
       </c>
       <c r="D29" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E29" s="31">
+        <f t="shared" si="1"/>
         <v>-0.9</v>
       </c>
       <c r="F29" s="53"/>
@@ -2727,13 +2785,16 @@
       <c r="B30" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C30" s="30">
+        <f t="shared" si="1"/>
         <v>-4.62</v>
       </c>
       <c r="D30" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E30" s="31">
+        <f t="shared" si="1"/>
         <v>-0.9</v>
       </c>
       <c r="F30" s="53"/>
@@ -2747,13 +2808,16 @@
       <c r="B31" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31" s="30">
+        <f t="shared" si="1"/>
         <v>-19.28</v>
       </c>
       <c r="D31" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E31" s="31">
+        <f t="shared" si="1"/>
         <v>-0.85099999999999998</v>
       </c>
       <c r="F31" s="53"/>
@@ -2767,9 +2831,18 @@
       <c r="B32" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
+      <c r="C32" s="30">
+        <f t="shared" si="1"/>
+        <v>-28.06</v>
+      </c>
+      <c r="D32" s="30">
+        <f t="shared" si="1"/>
+        <v>-7.5209999999999999</v>
+      </c>
+      <c r="E32" s="31">
+        <f t="shared" si="1"/>
+        <v>0.14099999999999999</v>
+      </c>
       <c r="F32" s="53"/>
       <c r="G32" s="53"/>
       <c r="H32" s="54"/>
@@ -2781,9 +2854,18 @@
       <c r="B33" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
+      <c r="C33" s="30">
+        <f t="shared" si="1"/>
+        <v>-28.06</v>
+      </c>
+      <c r="D33" s="30">
+        <f t="shared" si="1"/>
+        <v>7.5209999999999999</v>
+      </c>
+      <c r="E33" s="31">
+        <f t="shared" si="1"/>
+        <v>0.14099999999999999</v>
+      </c>
       <c r="F33" s="53"/>
       <c r="G33" s="53"/>
       <c r="H33" s="54"/>
@@ -2795,14 +2877,17 @@
       <c r="B34" s="56">
         <v>1442.64</v>
       </c>
-      <c r="C34" s="29">
+      <c r="C34" s="30">
+        <f t="shared" si="1"/>
         <v>-28.265099212856772</v>
       </c>
       <c r="D34" s="30">
+        <f t="shared" si="1"/>
         <v>-31.416080260883309</v>
       </c>
-      <c r="E34" s="31" t="s">
-        <v>37</v>
+      <c r="E34" s="31" t="str">
+        <f t="shared" ref="E34" si="2">E13</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
@@ -2816,14 +2901,17 @@
       <c r="B35" s="56">
         <v>1452.83</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="30">
+        <f t="shared" si="1"/>
         <v>-28.405576685387736</v>
       </c>
       <c r="D35" s="30">
+        <f t="shared" si="1"/>
         <v>31.763774206345854</v>
       </c>
-      <c r="E35" s="31" t="s">
-        <v>37</v>
+      <c r="E35" s="31" t="str">
+        <f t="shared" ref="E35" si="3">E14</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="32"/>
@@ -2837,13 +2925,16 @@
       <c r="B36" s="28">
         <v>95.85</v>
       </c>
-      <c r="C36" s="29">
+      <c r="C36" s="30">
+        <f t="shared" si="1"/>
         <v>-42.45</v>
       </c>
       <c r="D36" s="30">
+        <f t="shared" si="1"/>
         <v>-60.25</v>
       </c>
       <c r="E36" s="31">
+        <f t="shared" ref="E36" si="4">E15</f>
         <v>-0.2122</v>
       </c>
       <c r="F36" s="32"/>
@@ -2857,13 +2948,16 @@
       <c r="B37" s="28">
         <v>96.45</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="30">
+        <f t="shared" si="1"/>
         <v>-42.45</v>
       </c>
       <c r="D37" s="30">
+        <f t="shared" si="1"/>
         <v>60.25</v>
       </c>
       <c r="E37" s="31">
+        <f t="shared" si="1"/>
         <v>-0.2122</v>
       </c>
       <c r="F37" s="32"/>
@@ -2877,13 +2971,16 @@
       <c r="B38" s="28">
         <v>67.81</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="30">
+        <f t="shared" si="1"/>
         <v>-20.216666666666665</v>
       </c>
       <c r="D38" s="30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E38" s="31">
+        <f t="shared" si="1"/>
         <v>-0.15666666666666659</v>
       </c>
       <c r="F38" s="32"/>
@@ -2893,9 +2990,9 @@
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2944,4 +3041,633 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="2"/>
+      <c r="D1" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>42248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
+        <f>'Hati - Test Summary'!B19</f>
+        <v>6353.43</v>
+      </c>
+      <c r="D3" s="45">
+        <f>'Hati - Test Summary'!C19</f>
+        <v>-23.701232316402319</v>
+      </c>
+      <c r="E3" s="45">
+        <f>'Hati - Test Summary'!D19</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="45">
+        <f>'Hati - Test Summary'!E19</f>
+        <v>-0.4910901535076328</v>
+      </c>
+      <c r="G3" s="46">
+        <f>'Hati - Test Summary'!F19</f>
+        <v>2.7858559094921902</v>
+      </c>
+      <c r="H3" s="46">
+        <f>'Hati - Test Summary'!G19</f>
+        <v>0.48103970797577666</v>
+      </c>
+      <c r="I3" s="46">
+        <f>'Hati - Test Summary'!H19</f>
+        <v>3.063409536761633</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>42248</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="45">
+        <v>0</v>
+      </c>
+      <c r="E5" s="45">
+        <f>'Hati - Test Summary'!D8</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0</v>
+      </c>
+      <c r="G5" s="48">
+        <v>0</v>
+      </c>
+      <c r="H5" s="48">
+        <v>0</v>
+      </c>
+      <c r="I5" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="44"/>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f>C3+C5</f>
+        <v>6353.43</v>
+      </c>
+      <c r="D6" s="45">
+        <f>(D3*$C3 + D5*$C5)/$C6</f>
+        <v>-23.701232316402319</v>
+      </c>
+      <c r="E6" s="45">
+        <f t="shared" ref="E6:F6" si="0">(E3*$C3 + E5*$C5)/$C6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="45">
+        <f t="shared" si="0"/>
+        <v>-0.4910901535076328</v>
+      </c>
+      <c r="G6" s="46">
+        <f>(G3+($C3/1000)*(($E3*in2m-$E6*in2m)^2+($F3*in2m-$F6*in2m)^2)) + SIGN($C5)*((G5)+ABS($C5/1000)*(($E5*in2m-$E6*in2m)^2+($F5*in2m-$F6*in2m)^2))</f>
+        <v>2.7858559094921902</v>
+      </c>
+      <c r="H6" s="46">
+        <f>(H3+($C3/1000)*(($D3*in2m-$D6*in2m)^2+($F3*in2m-$F6*in2m)^2)) + SIGN($C5)*((H5)+ABS($C5/1000)*(($D5*in2m-$D6*in2m)^2+($F5*in2m-$F6*in2m)^2))</f>
+        <v>0.48103970797577666</v>
+      </c>
+      <c r="I6" s="46">
+        <f>(I3+($C3/1000)*(($D3*in2m-$D6*in2m)^2+($E3*in2m-$E6*in2m)^2)) + SIGN($C5)*((I5)+ABS($C5/1000)*(($D5*in2m-$D6*in2m)^2+($E5*in2m-$E6*in2m)^2))</f>
+        <v>3.063409536761633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="62">
+        <f>C6/1000*2.20462</f>
+        <v>14.0068988466</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="58" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="64"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="22">
+        <v>3362.34</v>
+      </c>
+      <c r="C6" s="23">
+        <v>-19.029243837922397</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
+        <v>-0.48787888524063588</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="29">
+        <v>-9.0624380999999996</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="31">
+        <v>-2.0267940000000002</v>
+      </c>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="54"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="29">
+        <v>-4.62</v>
+      </c>
+      <c r="D8" s="30">
+        <v>0</v>
+      </c>
+      <c r="E8" s="31">
+        <v>-0.61350000000000005</v>
+      </c>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="54"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="29">
+        <v>-4.62</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0</v>
+      </c>
+      <c r="E9" s="31">
+        <v>-0.35220000000000001</v>
+      </c>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="29">
+        <v>-19.28</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0</v>
+      </c>
+      <c r="E10" s="31">
+        <v>-0.85099999999999998</v>
+      </c>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="29">
+        <v>-28.06</v>
+      </c>
+      <c r="D11" s="30">
+        <v>-7.5209999999999999</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="29">
+        <v>-28.06</v>
+      </c>
+      <c r="D12" s="30">
+        <v>7.5209999999999999</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="54"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="28">
+        <v>1413.04</v>
+      </c>
+      <c r="C13" s="29">
+        <v>-28.927117339446426</v>
+      </c>
+      <c r="D13" s="30">
+        <v>-32.557770333736727</v>
+      </c>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="33"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="28">
+        <v>1429.75</v>
+      </c>
+      <c r="C14" s="29">
+        <v>-28.787806445537079</v>
+      </c>
+      <c r="D14" s="30">
+        <v>32.5466471670033</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="28">
+        <v>42.2</v>
+      </c>
+      <c r="C15" s="29">
+        <v>-42.448678000000001</v>
+      </c>
+      <c r="D15" s="30">
+        <v>-60.25</v>
+      </c>
+      <c r="E15" s="31">
+        <v>-0.2122</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="28">
+        <v>38.29</v>
+      </c>
+      <c r="C16" s="29">
+        <v>-42.448678000000001</v>
+      </c>
+      <c r="D16" s="30">
+        <v>60.25</v>
+      </c>
+      <c r="E16" s="31">
+        <v>-0.2122</v>
+      </c>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="28">
+        <v>67.81</v>
+      </c>
+      <c r="C17" s="29">
+        <v>-20.216666666666665</v>
+      </c>
+      <c r="D17" s="30">
+        <v>0</v>
+      </c>
+      <c r="E17" s="31">
+        <v>-0.15666666666666659</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="34">
+        <v>6353.43</v>
+      </c>
+      <c r="C19" s="35">
+        <v>-23.701232316402319</v>
+      </c>
+      <c r="D19" s="36">
+        <v>0</v>
+      </c>
+      <c r="E19" s="37">
+        <v>-0.4910901535076328</v>
+      </c>
+      <c r="F19" s="38">
+        <v>2.7858559094921902</v>
+      </c>
+      <c r="G19" s="38">
+        <v>0.48103970797577666</v>
+      </c>
+      <c r="H19" s="39">
+        <v>3.063409536761633</v>
+      </c>
+      <c r="I19" s="68">
+        <v>3.2435285669276975E-2</v>
+      </c>
+      <c r="J19" s="68">
+        <v>3.0177379598048133E-2</v>
+      </c>
+      <c r="K19" s="69">
+        <v>1.5725484307849608E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="57"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="43">
+        <f>B19/1000*2.20462</f>
+        <v>14.0068988466</v>
+      </c>
+      <c r="F21" s="40">
+        <f>F19*'Skoll - Test Summary'!$K$6</f>
+        <v>9519.7485263761882</v>
+      </c>
+      <c r="G21" s="41">
+        <f>G19*'Skoll - Test Summary'!$K$6</f>
+        <v>1643.7953720174878</v>
+      </c>
+      <c r="H21" s="42">
+        <f>H19*'Skoll - Test Summary'!$K$6</f>
+        <v>10468.196981727304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mass Properties update to denote flights
I added some of the flight numbers to the spreadsheet tracking Skoll's
mass properties.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Mass Properties.xlsx
+++ b/Design/CAD/mAEWing1 - Mass Properties.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>Left Wing</t>
   </si>
@@ -68,10 +68,6 @@
   </si>
   <si>
     <t>Summary Test Results</t>
-  </si>
-  <si>
-    <t>Flight Configuration for Flight1 and Flight2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Assume negligible body inertia</t>
@@ -244,6 +240,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Flight 3 and 4</t>
+  </si>
+  <si>
+    <t>Flight 1 and  2</t>
+  </si>
+  <si>
+    <t>Flight 6</t>
+  </si>
+  <si>
+    <t>Flight 9</t>
   </si>
 </sst>
 </file>
@@ -477,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -619,6 +627,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,18 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,11 +954,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,43 +966,43 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="2"/>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>12</v>
@@ -1004,7 +1013,7 @@
         <v>42161</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <f>'Skoll - Test Summary'!B19</f>
@@ -1071,13 +1080,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <f>C3+C5</f>
@@ -1119,7 +1128,7 @@
         <v>42161</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>-104.4</v>
@@ -1152,7 +1161,7 @@
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <f>C6+C8</f>
@@ -1194,7 +1203,7 @@
         <v>42166</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <f>23+8+16</f>
@@ -1220,13 +1229,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <f>C9+C11</f>
@@ -1268,7 +1277,7 @@
         <v>42166</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="47">
         <v>58</v>
@@ -1298,13 +1307,13 @@
         <v>4.8977777777777778E-4</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <f>C12+C14</f>
@@ -1343,7 +1352,7 @@
         <v>42170</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="47">
         <v>165</v>
@@ -1370,12 +1379,12 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <f>C15+C17</f>
@@ -1411,7 +1420,7 @@
         <v>42170</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="47">
         <v>-210.42</v>
@@ -1435,12 +1444,12 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <f>C18+C20</f>
@@ -1476,7 +1485,7 @@
         <v>42170</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="47">
         <v>546.64</v>
@@ -1503,12 +1512,12 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <f>C21+C23</f>
@@ -1574,12 +1583,12 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <f>C24+C26</f>
@@ -1615,7 +1624,7 @@
         <v>42177</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="47">
         <v>-55</v>
@@ -1642,12 +1651,12 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30">
         <f>C27+C29</f>
@@ -1683,7 +1692,7 @@
         <v>42177</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="47">
         <v>55</v>
@@ -1710,12 +1719,12 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>16</v>
       </c>
       <c r="C33">
         <f>C30+C32</f>
@@ -1745,16 +1754,16 @@
         <f>(I30+($C30/1000)*(($D30*in2m-$D33*in2m)^2+($E30*in2m-$E33*in2m)^2)) + SIGN($C32)*((I32)+ABS($C32/1000)*(($D32*in2m-$D33*in2m)^2+($E32*in2m-$E33*in2m)^2))</f>
         <v>3.287097144533309</v>
       </c>
-      <c r="J33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="44">
         <v>42186</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35">
         <v>68.02</v>
@@ -1778,12 +1787,12 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36">
         <f>C33+C35</f>
@@ -1814,12 +1823,12 @@
         <v>3.2872822730973268</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="44">
         <v>42186</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38">
         <v>119.55</v>
@@ -1843,51 +1852,54 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="47" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39">
+      <c r="C39" s="47">
         <f>C36+C38</f>
         <v>6684.8600000000015</v>
       </c>
-      <c r="D39" s="45">
+      <c r="D39" s="52">
         <f>(D36*$C36 + D38*$C38)/$C39</f>
         <v>-23.695628418545784</v>
       </c>
-      <c r="E39" s="45">
+      <c r="E39" s="52">
         <f t="shared" ref="E39:F39" si="19">(E36*$C36 + E38*$C38)/$C39</f>
         <v>-3.2910188096684147E-2</v>
       </c>
-      <c r="F39" s="45">
+      <c r="F39" s="52">
         <f t="shared" si="19"/>
         <v>-0.49769705274306414</v>
       </c>
-      <c r="G39" s="46">
+      <c r="G39" s="70">
         <f>(G36+($C36/1000)*(($E36*in2m-$E39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((G38)+ABS($C38/1000)*(($E38*in2m-$E39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
         <v>3.0986083814829324</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="70">
         <f>(H36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($F36*in2m-$F39*in2m)^2)) + SIGN($C38)*((H38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($F38*in2m-$F39*in2m)^2))</f>
         <v>0.52818416630470488</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="70">
         <f>(I36+($C36/1000)*(($D36*in2m-$D39*in2m)^2+($E36*in2m-$E39*in2m)^2)) + SIGN($C38)*((I38)+ABS($C38/1000)*(($D38*in2m-$D39*in2m)^2+($E38*in2m-$E39*in2m)^2))</f>
         <v>3.3158590400713943</v>
       </c>
       <c r="J39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="44">
         <v>42217</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41">
         <f>-C32</f>
@@ -1918,12 +1930,12 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>16</v>
       </c>
       <c r="C42">
         <f>C39+C41</f>
@@ -1954,12 +1966,12 @@
         <v>3.3147385180444222</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="44">
         <v>42217</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44">
         <v>96</v>
@@ -1985,12 +1997,12 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C45">
         <f>C42+C44</f>
@@ -2021,12 +2033,12 @@
         <v>3.3251924426702351</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="44">
         <v>42217</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47">
         <f>49-121</f>
@@ -2051,12 +2063,12 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>16</v>
       </c>
       <c r="C48">
         <f>C45+C47</f>
@@ -2087,15 +2099,18 @@
         <v>3.3084221160314553</v>
       </c>
       <c r="J48" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="44">
         <v>42225</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50">
         <v>40</v>
@@ -2121,12 +2136,12 @@
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C51">
         <f>C48+C50</f>
@@ -2157,12 +2172,12 @@
         <v>3.3094327470082918</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="44">
         <v>42225</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53">
         <v>15</v>
@@ -2186,12 +2201,12 @@
         <v>0</v>
       </c>
       <c r="J53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>16</v>
       </c>
       <c r="C54">
         <f>C51+C53</f>
@@ -2222,10 +2237,13 @@
         <v>3.3129703252740588</v>
       </c>
       <c r="J54" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C57" s="62">
         <f>C48/1000*2.20462</f>
         <v>14.669232833200002</v>
@@ -2254,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,7 +2284,7 @@
   <sheetData>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2274,57 +2292,57 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="69"/>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="18">
         <v>9.8066499999999994</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="20">
         <v>2.5399999999999999E-2</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2350,7 +2368,7 @@
         <v>0.14448048825940063</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="20">
@@ -2360,10 +2378,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>61</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>62</v>
       </c>
       <c r="C7" s="29">
         <v>-9.0909999999999993</v>
@@ -2406,10 +2424,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="29">
         <v>-4.62</v>
@@ -2426,10 +2444,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="29">
         <v>-19.28</v>
@@ -2446,10 +2464,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="29">
         <v>-28.06</v>
@@ -2466,10 +2484,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="29">
         <v>-28.06</v>
@@ -2498,7 +2516,7 @@
         <v>-31.416080260883309</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
@@ -2518,7 +2536,7 @@
         <v>31.763774206345854</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
@@ -2596,7 +2614,7 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="34">
         <v>6269.81</v>
@@ -2625,7 +2643,7 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="43">
         <f>B19/1000*2.20462</f>
@@ -2660,7 +2678,7 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2668,39 +2686,39 @@
         <v>10</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="64"/>
-      <c r="H25" s="65"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="69"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="E26" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="F26" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="G26" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="H26" s="51" t="s">
         <v>32</v>
-      </c>
-      <c r="H26" s="51" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2728,10 +2746,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="30">
         <f t="shared" ref="C28:E38" si="1">C7</f>
@@ -2760,7 +2778,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="30">
         <f t="shared" si="1"/>
@@ -2780,10 +2798,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="30">
         <f t="shared" si="1"/>
@@ -2803,10 +2821,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="30">
         <f t="shared" si="1"/>
@@ -2826,10 +2844,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="30">
         <f t="shared" si="1"/>
@@ -2849,10 +2867,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="30">
         <f t="shared" si="1"/>
@@ -2999,7 +3017,7 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="34">
         <f>SUM(B27:B39)</f>
@@ -3015,7 +3033,7 @@
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="43">
         <f>B40/1000*2.20462</f>
@@ -3062,38 +3080,38 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="2"/>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="65"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="F2" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G2" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="H2" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="I2" s="51" t="s">
         <v>32</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>33</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>12</v>
@@ -3104,7 +3122,7 @@
         <v>42248</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3">
         <f>'Hati - Test Summary'!B19</f>
@@ -3143,7 +3161,7 @@
         <v>42248</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -3171,7 +3189,7 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <f>C3+C5</f>
@@ -3246,7 +3264,7 @@
   <sheetData>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3254,53 +3272,53 @@
         <v>10</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="65"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15"/>
       <c r="B5" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="E5" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="F5" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="G5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="H5" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="51" t="s">
-        <v>33</v>
-      </c>
       <c r="I5" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="50" t="s">
+      <c r="K5" s="51" t="s">
         <v>32</v>
-      </c>
-      <c r="K5" s="51" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3322,16 +3340,16 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="27"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
       <c r="K6" s="27"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="29">
         <v>-9.0624380999999996</v>
@@ -3345,8 +3363,8 @@
       <c r="F7" s="53"/>
       <c r="G7" s="53"/>
       <c r="H7" s="54"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
       <c r="K7" s="54"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3354,7 +3372,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="29">
         <v>-4.62</v>
@@ -3374,10 +3392,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="29">
         <v>-4.62</v>
@@ -3397,10 +3415,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="29">
         <v>-19.28</v>
@@ -3420,10 +3438,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="29">
         <v>-28.06</v>
@@ -3443,10 +3461,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="29">
         <v>-28.06</v>
@@ -3590,7 +3608,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="34">
         <v>6353.43</v>
@@ -3613,13 +3631,13 @@
       <c r="H19" s="39">
         <v>3.063409536761633</v>
       </c>
-      <c r="I19" s="68">
+      <c r="I19" s="65">
         <v>3.2435285669276975E-2</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="65">
         <v>3.0177379598048133E-2</v>
       </c>
-      <c r="K19" s="69">
+      <c r="K19" s="66">
         <v>1.5725484307849608E-2</v>
       </c>
     </row>
@@ -3628,7 +3646,7 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="43">
         <f>B19/1000*2.20462</f>

</xml_diff>